<commit_message>
New component cost capex. opex remaining
</commit_message>
<xml_diff>
--- a/tumlknexpectimax/excel_data/input_data_residential.xlsx
+++ b/tumlknexpectimax/excel_data/input_data_residential.xlsx
@@ -1,15 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="18431"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ahmadzay\PycharmProjects\mt_code\tumlknexpectimax\tumlknexpectimax\excel_data\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="480" yWindow="768" windowWidth="15108" windowHeight="8688" activeTab="1"/>
+    <workbookView xWindow="480" yWindow="885" windowWidth="15105" windowHeight="8565" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="CAPEX" sheetId="1" r:id="rId1"/>
@@ -31,7 +26,7 @@
     <sheet name="FTTB_Hybridpon_100" sheetId="19" r:id="rId17"/>
     <sheet name="MIG_MATRIX" sheetId="11" r:id="rId18"/>
   </sheets>
-  <calcPr calcId="171027"/>
+  <calcPr calcId="145621"/>
 </workbook>
 </file>
 
@@ -41,7 +36,7 @@
     <author>Patri, Sai Kireet</author>
   </authors>
   <commentList>
-    <comment ref="B3" authorId="0" shapeId="0">
+    <comment ref="B3" authorId="0">
       <text>
         <r>
           <rPr>
@@ -66,7 +61,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="G4" authorId="0" shapeId="0">
+    <comment ref="G4" authorId="0">
       <text>
         <r>
           <rPr>
@@ -92,7 +87,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="G5" authorId="0" shapeId="0">
+    <comment ref="G5" authorId="0">
       <text>
         <r>
           <rPr>
@@ -116,7 +111,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="G6" authorId="0" shapeId="0">
+    <comment ref="G6" authorId="0">
       <text>
         <r>
           <rPr>
@@ -141,7 +136,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="G7" authorId="0" shapeId="0">
+    <comment ref="G7" authorId="0">
       <text>
         <r>
           <rPr>
@@ -166,7 +161,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B8" authorId="0" shapeId="0">
+    <comment ref="B8" authorId="0">
       <text>
         <r>
           <rPr>
@@ -441,7 +436,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.00000000000%"/>
   </numFmts>
@@ -612,7 +607,7 @@
     <xf numFmtId="0" fontId="7" fillId="4" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="8" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -625,6 +620,7 @@
     <xf numFmtId="0" fontId="7" fillId="4" borderId="2" xfId="6"/>
     <xf numFmtId="0" fontId="6" fillId="4" borderId="3" xfId="5"/>
     <xf numFmtId="0" fontId="8" fillId="5" borderId="0" xfId="7"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="8">
     <cellStyle name="Calculation" xfId="6" builtinId="22"/>
@@ -642,17 +638,14 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
   </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
+  <c:lang val="de-DE"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -679,6 +672,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="1"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -757,48 +751,48 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="13"/>
                 <c:pt idx="0">
-                  <c:v>146337.87420813384</c:v>
+                  <c:v>146337.9</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>146337.87420813384</c:v>
+                  <c:v>146337.9</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>78872.086550701642</c:v>
+                  <c:v>78872.09</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>78872.086550701642</c:v>
+                  <c:v>78872.09</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>146337.87420813384</c:v>
+                  <c:v>146337.9</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>146337.87420813384</c:v>
+                  <c:v>146337.9</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>146337.87420813384</c:v>
+                  <c:v>146337.9</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>78872.086550701642</c:v>
+                  <c:v>78872.09</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>114876.35990534152</c:v>
+                  <c:v>114876.4</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>115530.46906962365</c:v>
+                  <c:v>115530.5</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>115530.46906962365</c:v>
+                  <c:v>115530.5</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>114876.35990534152</c:v>
+                  <c:v>114876.4</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>115530.46906962365</c:v>
+                  <c:v>115530.5</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000000-37DD-494B-898C-2092A609AD86}"/>
             </c:ext>
@@ -873,48 +867,48 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="13"/>
                 <c:pt idx="0">
-                  <c:v>18.840228189119191</c:v>
+                  <c:v>18.840229999999998</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>12.814589886676153</c:v>
+                  <c:v>12.814590000000001</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>14.612123172178348</c:v>
+                  <c:v>14.612120000000001</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>14.612123172178348</c:v>
+                  <c:v>14.612120000000001</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>12.814589886676153</c:v>
+                  <c:v>12.814590000000001</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>18.840228189119191</c:v>
+                  <c:v>18.840229999999998</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>12.814589886676153</c:v>
+                  <c:v>12.814590000000001</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>14.612123172178348</c:v>
+                  <c:v>14.612120000000001</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>12.594228370284263</c:v>
+                  <c:v>12.59423</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>12.211670303203721</c:v>
+                  <c:v>12.21167</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>25.08727030320372</c:v>
+                  <c:v>25.08727</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>12.594228370284263</c:v>
+                  <c:v>12.59423</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>12.211670303203721</c:v>
+                  <c:v>12.21167</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000001-37DD-494B-898C-2092A609AD86}"/>
             </c:ext>
@@ -989,48 +983,48 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="13"/>
                 <c:pt idx="0">
-                  <c:v>1717.1200000000001</c:v>
+                  <c:v>3056.8888888888887</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1609.5</c:v>
+                  <c:v>6405.333333333333</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>6330.7</c:v>
+                  <c:v>5299.166666666667</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>21352.036666666667</c:v>
+                  <c:v>5866.833333333333</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>9656.6999999999989</c:v>
+                  <c:v>12618.666666666666</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>6974.5</c:v>
+                  <c:v>6426.666666666667</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>3862.7999999999997</c:v>
+                  <c:v>12818.666666666666</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>6438</c:v>
+                  <c:v>5866.833333333333</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>966.06000000000006</c:v>
+                  <c:v>4000</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>1502.2</c:v>
+                  <c:v>7280</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>17382.060000000001</c:v>
+                  <c:v>14160</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>2897.1000000000004</c:v>
+                  <c:v>14800</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>2897.1000000000004</c:v>
+                  <c:v>14160</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000002-37DD-494B-898C-2092A609AD86}"/>
             </c:ext>
@@ -1105,48 +1099,48 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="13"/>
                 <c:pt idx="0">
-                  <c:v>5044.04</c:v>
+                  <c:v>192395.6</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>12768.7</c:v>
+                  <c:v>62262.5</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>11588.4</c:v>
+                  <c:v>59401.22</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>107189.37</c:v>
+                  <c:v>72078.600000000006</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>76609.820000000007</c:v>
+                  <c:v>68200.2</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>13841.7</c:v>
+                  <c:v>195086.4</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>14700.099999999999</c:v>
+                  <c:v>61989.9</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>11588.4</c:v>
+                  <c:v>61547.1</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>4436.72</c:v>
+                  <c:v>96145</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>17919.099999999999</c:v>
+                  <c:v>55966.5</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>108798.82</c:v>
+                  <c:v>106486.5</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>13305.200000000003</c:v>
+                  <c:v>105356</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>18133.7</c:v>
+                  <c:v>56966.5</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000003-37DD-494B-898C-2092A609AD86}"/>
             </c:ext>
@@ -1162,11 +1156,11 @@
         </c:dLbls>
         <c:gapWidth val="150"/>
         <c:overlap val="100"/>
-        <c:axId val="173921024"/>
-        <c:axId val="173922944"/>
+        <c:axId val="157322240"/>
+        <c:axId val="174832960"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="173921024"/>
+        <c:axId val="157322240"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1188,13 +1182,14 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="0"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="173922944"/>
+        <c:crossAx val="174832960"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1202,7 +1197,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="173922944"/>
+        <c:axId val="174832960"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1225,19 +1220,21 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="173921024"/>
+        <c:crossAx val="157322240"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -1253,9 +1250,9 @@
 </file>
 
 <file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
+  <c:lang val="de-DE"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -1267,6 +1264,7 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -1315,21 +1313,21 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>146337.87420813384</c:v>
+                  <c:v>146337.9</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>18.840228189119191</c:v>
+                  <c:v>18.840229999999998</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1717.1200000000001</c:v>
+                  <c:v>3056.8888888888887</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>5044.04</c:v>
+                  <c:v>192395.6</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000000-CEE8-43A2-851D-BC93CBA0BE7C}"/>
             </c:ext>
@@ -1349,6 +1347,7 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:txPr>
         <a:bodyPr/>
@@ -1357,7 +1356,7 @@
           <a:pPr rtl="0">
             <a:defRPr/>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="de-DE"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -1374,9 +1373,9 @@
 </file>
 
 <file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
+  <c:lang val="de-DE"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -1403,6 +1402,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -1484,51 +1484,51 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="14"/>
                 <c:pt idx="0">
-                  <c:v>2500</c:v>
+                  <c:v>11239.427296319658</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2139.68314436323</c:v>
+                  <c:v>21008.816291188887</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>2901.3268879802054</c:v>
+                  <c:v>8330.290479233332</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>2580.7769867387378</c:v>
+                  <c:v>7258.905687866667</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>13643.007653405404</c:v>
+                  <c:v>8583.4103545333346</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>10090.158887980206</c:v>
+                  <c:v>9545.3938125666664</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>3545.1871443632299</c:v>
+                  <c:v>21614.874068966667</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>3319.7968879802052</c:v>
+                  <c:v>8944.3638125666657</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>2591.5069867387383</c:v>
+                  <c:v>7530.2603545333332</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>1689.1675413371181</c:v>
+                  <c:v>11163.3899423</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>3097.556807399269</c:v>
+                  <c:v>7480.0771167000003</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>13773.64356339927</c:v>
+                  <c:v>13220.205872700002</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>2769.1195413371188</c:v>
+                  <c:v>13164.489942300001</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>3258.5068073992688</c:v>
+                  <c:v>8268.0771167000003</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000000-B8F6-416E-AD21-7DE814CEBF97}"/>
             </c:ext>
@@ -1543,11 +1543,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="174888832"/>
-        <c:axId val="174890368"/>
+        <c:axId val="179649536"/>
+        <c:axId val="179948352"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="174888832"/>
+        <c:axId val="179649536"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1557,7 +1557,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="174890368"/>
+        <c:crossAx val="179948352"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1565,7 +1565,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="174890368"/>
+        <c:axId val="179948352"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1588,13 +1588,14 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="174888832"/>
+        <c:crossAx val="179649536"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1612,9 +1613,9 @@
 </file>
 
 <file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
+  <c:lang val="de-DE"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -1626,6 +1627,7 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -1743,7 +1745,7 @@
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000000-DDCA-4663-830D-82651783C711}"/>
             </c:ext>
@@ -1758,11 +1760,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="174947712"/>
-        <c:axId val="174958080"/>
+        <c:axId val="172711936"/>
+        <c:axId val="179950080"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="174947712"/>
+        <c:axId val="172711936"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1784,13 +1786,14 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="0"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="174958080"/>
+        <c:crossAx val="179950080"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1798,7 +1801,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="174958080"/>
+        <c:axId val="179950080"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1821,13 +1824,14 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="174947712"/>
+        <c:crossAx val="172711936"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1845,9 +1849,9 @@
 </file>
 
 <file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
+  <c:lang val="de-DE"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -2024,7 +2028,7 @@
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000000-B323-4672-88DD-A4269C32C76F}"/>
             </c:ext>
@@ -2189,7 +2193,7 @@
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000001-B323-4672-88DD-A4269C32C76F}"/>
             </c:ext>
@@ -2354,7 +2358,7 @@
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000002-B323-4672-88DD-A4269C32C76F}"/>
             </c:ext>
@@ -2369,11 +2373,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="175550464"/>
-        <c:axId val="175552000"/>
+        <c:axId val="174748160"/>
+        <c:axId val="179951808"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="175550464"/>
+        <c:axId val="174748160"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2383,7 +2387,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="175552000"/>
+        <c:crossAx val="179951808"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2391,7 +2395,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="175552000"/>
+        <c:axId val="179951808"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2402,7 +2406,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="175550464"/>
+        <c:crossAx val="174748160"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2443,7 +2447,7 @@
         <xdr:cNvPr id="5" name="Chart 4">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000005000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000005000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2479,7 +2483,7 @@
         <xdr:cNvPr id="2" name="Chart 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000002000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2504,23 +2508,23 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>361949</xdr:colOff>
-      <xdr:row>15</xdr:row>
-      <xdr:rowOff>161925</xdr:rowOff>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>438150</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>13</xdr:col>
-      <xdr:colOff>209549</xdr:colOff>
-      <xdr:row>43</xdr:row>
-      <xdr:rowOff>161925</xdr:rowOff>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>266700</xdr:colOff>
+      <xdr:row>46</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="2" name="Chart 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000002000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2556,7 +2560,7 @@
         <xdr:cNvPr id="3" name="Chart 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000003000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000003000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2597,7 +2601,7 @@
         <xdr:cNvPr id="2" name="Chart 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0800-000002000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0800-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2661,7 +2665,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -2694,26 +2698,9 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -2746,23 +2733,6 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -2941,31 +2911,31 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Y65"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+    <sheetView topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="V9" sqref="V9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="29.44140625" customWidth="1"/>
-    <col min="2" max="2" width="18.6640625" customWidth="1"/>
-    <col min="3" max="3" width="18.33203125" customWidth="1"/>
-    <col min="4" max="4" width="15.109375" customWidth="1"/>
-    <col min="5" max="5" width="13.44140625" customWidth="1"/>
-    <col min="6" max="6" width="13.5546875" customWidth="1"/>
-    <col min="7" max="7" width="17.44140625" customWidth="1"/>
-    <col min="8" max="9" width="19.109375" customWidth="1"/>
+    <col min="1" max="1" width="29.42578125" customWidth="1"/>
+    <col min="2" max="2" width="18.7109375" customWidth="1"/>
+    <col min="3" max="3" width="18.28515625" customWidth="1"/>
+    <col min="4" max="4" width="15.140625" customWidth="1"/>
+    <col min="5" max="5" width="13.42578125" customWidth="1"/>
+    <col min="6" max="6" width="13.5703125" customWidth="1"/>
+    <col min="7" max="7" width="17.42578125" customWidth="1"/>
+    <col min="8" max="9" width="19.140625" customWidth="1"/>
     <col min="10" max="10" width="14" customWidth="1"/>
-    <col min="11" max="11" width="13.44140625" customWidth="1"/>
-    <col min="12" max="12" width="16.6640625" customWidth="1"/>
-    <col min="13" max="13" width="16.44140625" customWidth="1"/>
-    <col min="14" max="14" width="22.109375" customWidth="1"/>
-    <col min="15" max="15" width="13.5546875" customWidth="1"/>
-    <col min="16" max="17" width="11.6640625" customWidth="1"/>
-    <col min="23" max="23" width="13.44140625" customWidth="1"/>
+    <col min="11" max="11" width="13.42578125" customWidth="1"/>
+    <col min="12" max="12" width="16.7109375" customWidth="1"/>
+    <col min="13" max="13" width="16.42578125" customWidth="1"/>
+    <col min="14" max="14" width="22.140625" customWidth="1"/>
+    <col min="15" max="15" width="13.5703125" customWidth="1"/>
+    <col min="16" max="17" width="11.7109375" customWidth="1"/>
+    <col min="23" max="23" width="13.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:23" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
@@ -3036,7 +3006,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="2" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A2" s="7" t="s">
         <v>24</v>
       </c>
@@ -3069,11 +3039,11 @@
       <c r="T2" s="9"/>
       <c r="U2" s="9"/>
       <c r="V2" s="9">
-        <v>10000</v>
+        <v>100000</v>
       </c>
       <c r="W2" s="10"/>
     </row>
-    <row r="3" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A3" s="7" t="s">
         <v>65</v>
       </c>
@@ -3128,32 +3098,28 @@
       <c r="Q3" s="8">
         <v>685372.28279667499</v>
       </c>
-      <c r="R3" s="9">
-        <f t="shared" ref="R3:R15" si="0">L3*$R$46+M3*$S$46+N3*$V$46</f>
-        <v>146337.87420813384</v>
-      </c>
-      <c r="S3" s="9">
-        <f t="shared" ref="S3:S15" si="1">(O3+P3+Q3)*$P$27</f>
-        <v>18.840228189119191</v>
-      </c>
-      <c r="T3" s="9">
-        <f t="shared" ref="T3:T15" si="2">G3*B3</f>
-        <v>1717.1200000000001</v>
-      </c>
-      <c r="U3" s="9">
-        <f t="shared" ref="U3:U15" si="3">B3*H3+B3*I3</f>
-        <v>5044.04</v>
+      <c r="R3" s="12">
+        <v>146337.9</v>
+      </c>
+      <c r="S3" s="12">
+        <v>18.840229999999998</v>
+      </c>
+      <c r="T3" s="12">
+        <v>3056.8888888888887</v>
+      </c>
+      <c r="U3" s="12">
+        <v>192395.6</v>
       </c>
       <c r="V3" s="9">
-        <f t="shared" ref="V3:V15" si="4">SUM(T3,U3)</f>
-        <v>6761.16</v>
+        <f>SUM(T3,U3)</f>
+        <v>195452.48888888888</v>
       </c>
       <c r="W3" s="10">
-        <f t="shared" ref="W3:W15" si="5">R3+S3+T3+U3</f>
-        <v>153117.87443632298</v>
-      </c>
-    </row>
-    <row r="4" spans="1:23" x14ac:dyDescent="0.3">
+        <f>R3+S3+T3+U3</f>
+        <v>341809.22911888885</v>
+      </c>
+    </row>
+    <row r="4" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A4" s="7" t="s">
         <v>66</v>
       </c>
@@ -3208,32 +3174,28 @@
       <c r="Q4" s="8">
         <v>384090.36767452297</v>
       </c>
-      <c r="R4" s="9">
-        <f t="shared" si="0"/>
-        <v>146337.87420813384</v>
-      </c>
-      <c r="S4" s="9">
-        <f t="shared" si="1"/>
-        <v>12.814589886676153</v>
-      </c>
-      <c r="T4" s="9">
-        <f t="shared" si="2"/>
-        <v>1609.5</v>
-      </c>
-      <c r="U4" s="9">
-        <f t="shared" si="3"/>
-        <v>12768.7</v>
+      <c r="R4" s="12">
+        <v>146337.9</v>
+      </c>
+      <c r="S4" s="12">
+        <v>12.814590000000001</v>
+      </c>
+      <c r="T4" s="12">
+        <v>6405.333333333333</v>
+      </c>
+      <c r="U4" s="12">
+        <v>62262.5</v>
       </c>
       <c r="V4" s="9">
-        <f t="shared" si="4"/>
-        <v>14378.2</v>
+        <f t="shared" ref="V4:V15" si="0">SUM(T4,U4)</f>
+        <v>68667.833333333328</v>
       </c>
       <c r="W4" s="10">
-        <f t="shared" si="5"/>
-        <v>160728.88879802052</v>
-      </c>
-    </row>
-    <row r="5" spans="1:23" x14ac:dyDescent="0.3">
+        <f t="shared" ref="W4:W15" si="1">R4+S4+T4+U4</f>
+        <v>215018.54792333333</v>
+      </c>
+    </row>
+    <row r="5" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A5" s="7" t="s">
         <v>67</v>
       </c>
@@ -3284,32 +3246,28 @@
       <c r="Q5" s="8">
         <v>658286.15266324603</v>
       </c>
-      <c r="R5" s="9">
+      <c r="R5" s="12">
+        <v>78872.09</v>
+      </c>
+      <c r="S5" s="12">
+        <v>14.612120000000001</v>
+      </c>
+      <c r="T5" s="12">
+        <v>5299.166666666667</v>
+      </c>
+      <c r="U5" s="12">
+        <v>59401.22</v>
+      </c>
+      <c r="V5" s="9">
         <f t="shared" si="0"/>
-        <v>78872.086550701642</v>
-      </c>
-      <c r="S5" s="9">
+        <v>64700.386666666665</v>
+      </c>
+      <c r="W5" s="10">
         <f t="shared" si="1"/>
-        <v>14.612123172178348</v>
-      </c>
-      <c r="T5" s="9">
-        <f t="shared" si="2"/>
-        <v>6330.7</v>
-      </c>
-      <c r="U5" s="9">
-        <f t="shared" si="3"/>
-        <v>11588.4</v>
-      </c>
-      <c r="V5" s="9">
-        <f t="shared" si="4"/>
-        <v>17919.099999999999</v>
-      </c>
-      <c r="W5" s="10">
-        <f t="shared" si="5"/>
-        <v>96805.798673873811</v>
-      </c>
-    </row>
-    <row r="6" spans="1:23" x14ac:dyDescent="0.3">
+        <v>143587.08878666669</v>
+      </c>
+    </row>
+    <row r="6" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A6" s="7" t="s">
         <v>68</v>
       </c>
@@ -3364,32 +3322,28 @@
       <c r="Q6" s="8">
         <v>658286.15266324603</v>
       </c>
-      <c r="R6" s="9">
+      <c r="R6" s="12">
+        <v>78872.09</v>
+      </c>
+      <c r="S6" s="12">
+        <v>14.612120000000001</v>
+      </c>
+      <c r="T6" s="12">
+        <v>5866.833333333333</v>
+      </c>
+      <c r="U6" s="12">
+        <v>72078.600000000006</v>
+      </c>
+      <c r="V6" s="9">
         <f t="shared" si="0"/>
-        <v>78872.086550701642</v>
-      </c>
-      <c r="S6" s="9">
+        <v>77945.433333333334</v>
+      </c>
+      <c r="W6" s="10">
         <f t="shared" si="1"/>
-        <v>14.612123172178348</v>
-      </c>
-      <c r="T6" s="9">
-        <f t="shared" si="2"/>
-        <v>21352.036666666667</v>
-      </c>
-      <c r="U6" s="9">
-        <f t="shared" si="3"/>
-        <v>107189.37</v>
-      </c>
-      <c r="V6" s="9">
-        <f t="shared" si="4"/>
-        <v>128541.40666666666</v>
-      </c>
-      <c r="W6" s="10">
-        <f t="shared" si="5"/>
-        <v>207428.10534054047</v>
-      </c>
-    </row>
-    <row r="7" spans="1:23" x14ac:dyDescent="0.3">
+        <v>156832.13545333332</v>
+      </c>
+    </row>
+    <row r="7" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A7" s="7" t="s">
         <v>69</v>
       </c>
@@ -3444,32 +3398,28 @@
       <c r="Q7" s="8">
         <v>384090.36767452297</v>
       </c>
-      <c r="R7" s="9">
+      <c r="R7" s="12">
+        <v>146337.9</v>
+      </c>
+      <c r="S7" s="12">
+        <v>12.814590000000001</v>
+      </c>
+      <c r="T7" s="12">
+        <v>12618.666666666666</v>
+      </c>
+      <c r="U7" s="12">
+        <v>68200.2</v>
+      </c>
+      <c r="V7" s="9">
         <f t="shared" si="0"/>
-        <v>146337.87420813384</v>
-      </c>
-      <c r="S7" s="9">
+        <v>80818.866666666669</v>
+      </c>
+      <c r="W7" s="10">
         <f t="shared" si="1"/>
-        <v>12.814589886676153</v>
-      </c>
-      <c r="T7" s="9">
-        <f t="shared" si="2"/>
-        <v>9656.6999999999989</v>
-      </c>
-      <c r="U7" s="9">
-        <f t="shared" si="3"/>
-        <v>76609.820000000007</v>
-      </c>
-      <c r="V7" s="9">
-        <f t="shared" si="4"/>
-        <v>86266.52</v>
-      </c>
-      <c r="W7" s="10">
-        <f t="shared" si="5"/>
-        <v>232617.20879802053</v>
-      </c>
-    </row>
-    <row r="8" spans="1:23" x14ac:dyDescent="0.3">
+        <v>227169.58125666663</v>
+      </c>
+    </row>
+    <row r="8" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A8" s="7" t="s">
         <v>70</v>
       </c>
@@ -3499,10 +3449,10 @@
         <v>1</v>
       </c>
       <c r="J8" s="8">
-        <v>19</v>
+        <v>156</v>
       </c>
       <c r="K8" s="8">
-        <v>151</v>
+        <v>1244</v>
       </c>
       <c r="L8" s="8">
         <v>31505.122417993502</v>
@@ -3522,37 +3472,33 @@
       <c r="Q8" s="8">
         <v>685372.28279667499</v>
       </c>
-      <c r="R8" s="9">
+      <c r="R8" s="12">
+        <v>146337.9</v>
+      </c>
+      <c r="S8" s="12">
+        <v>18.840229999999998</v>
+      </c>
+      <c r="T8" s="12">
+        <v>6426.666666666667</v>
+      </c>
+      <c r="U8" s="12">
+        <v>195086.4</v>
+      </c>
+      <c r="V8" s="9">
         <f t="shared" si="0"/>
-        <v>146337.87420813384</v>
-      </c>
-      <c r="S8" s="9">
+        <v>201513.06666666665</v>
+      </c>
+      <c r="W8" s="10">
         <f t="shared" si="1"/>
-        <v>18.840228189119191</v>
-      </c>
-      <c r="T8" s="9">
-        <f t="shared" si="2"/>
-        <v>6974.5</v>
-      </c>
-      <c r="U8" s="9">
-        <f t="shared" si="3"/>
-        <v>13841.7</v>
-      </c>
-      <c r="V8" s="9">
-        <f t="shared" si="4"/>
-        <v>20816.2</v>
-      </c>
-      <c r="W8" s="10">
-        <f t="shared" si="5"/>
-        <v>167172.91443632299</v>
-      </c>
-    </row>
-    <row r="9" spans="1:23" x14ac:dyDescent="0.3">
+        <v>347869.80689666665</v>
+      </c>
+    </row>
+    <row r="9" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A9" s="7" t="s">
         <v>71</v>
       </c>
       <c r="B9" s="8">
-        <f t="shared" ref="B9:B15" si="6">CEILING(4877+0.1*(4877),1)</f>
+        <f t="shared" ref="B9:B15" si="2">CEILING(4877+0.1*(4877),1)</f>
         <v>5365</v>
       </c>
       <c r="C9" s="8">
@@ -3600,37 +3546,33 @@
       <c r="Q9" s="8">
         <v>384090.36767452297</v>
       </c>
-      <c r="R9" s="9">
+      <c r="R9" s="12">
+        <v>146337.9</v>
+      </c>
+      <c r="S9" s="12">
+        <v>12.814590000000001</v>
+      </c>
+      <c r="T9" s="12">
+        <v>12818.666666666666</v>
+      </c>
+      <c r="U9" s="12">
+        <v>61989.9</v>
+      </c>
+      <c r="V9" s="9">
         <f t="shared" si="0"/>
-        <v>146337.87420813384</v>
-      </c>
-      <c r="S9" s="9">
+        <v>74808.566666666666</v>
+      </c>
+      <c r="W9" s="10">
         <f t="shared" si="1"/>
-        <v>12.814589886676153</v>
-      </c>
-      <c r="T9" s="9">
-        <f t="shared" si="2"/>
-        <v>3862.7999999999997</v>
-      </c>
-      <c r="U9" s="9">
-        <f t="shared" si="3"/>
-        <v>14700.099999999999</v>
-      </c>
-      <c r="V9" s="9">
-        <f t="shared" si="4"/>
-        <v>18562.899999999998</v>
-      </c>
-      <c r="W9" s="10">
-        <f t="shared" si="5"/>
-        <v>164913.5887980205</v>
-      </c>
-    </row>
-    <row r="10" spans="1:23" x14ac:dyDescent="0.3">
+        <v>221159.28125666664</v>
+      </c>
+    </row>
+    <row r="10" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A10" s="7" t="s">
         <v>72</v>
       </c>
       <c r="B10" s="8">
-        <f t="shared" si="6"/>
+        <f t="shared" si="2"/>
         <v>5365</v>
       </c>
       <c r="C10" s="8">
@@ -3677,32 +3619,28 @@
       <c r="Q10" s="8">
         <v>658286.15266324603</v>
       </c>
-      <c r="R10" s="9">
+      <c r="R10" s="12">
+        <v>78872.09</v>
+      </c>
+      <c r="S10" s="12">
+        <v>14.612120000000001</v>
+      </c>
+      <c r="T10" s="12">
+        <v>5866.833333333333</v>
+      </c>
+      <c r="U10" s="12">
+        <v>61547.1</v>
+      </c>
+      <c r="V10" s="9">
         <f t="shared" si="0"/>
-        <v>78872.086550701642</v>
-      </c>
-      <c r="S10" s="9">
+        <v>67413.933333333334</v>
+      </c>
+      <c r="W10" s="10">
         <f t="shared" si="1"/>
-        <v>14.612123172178348</v>
-      </c>
-      <c r="T10" s="9">
-        <f t="shared" si="2"/>
-        <v>6438</v>
-      </c>
-      <c r="U10" s="9">
-        <f t="shared" si="3"/>
-        <v>11588.4</v>
-      </c>
-      <c r="V10" s="9">
-        <f t="shared" si="4"/>
-        <v>18026.400000000001</v>
-      </c>
-      <c r="W10" s="10">
-        <f t="shared" si="5"/>
-        <v>96913.098673873814</v>
-      </c>
-    </row>
-    <row r="11" spans="1:23" x14ac:dyDescent="0.3">
+        <v>146300.63545333332</v>
+      </c>
+    </row>
+    <row r="11" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A11" s="7" t="s">
         <v>73</v>
       </c>
@@ -3755,37 +3693,33 @@
       <c r="Q11" s="8">
         <v>387592.626526276</v>
       </c>
-      <c r="R11" s="9">
+      <c r="R11" s="12">
+        <v>114876.4</v>
+      </c>
+      <c r="S11" s="12">
+        <v>12.59423</v>
+      </c>
+      <c r="T11" s="12">
+        <v>4000</v>
+      </c>
+      <c r="U11" s="12">
+        <v>96145</v>
+      </c>
+      <c r="V11" s="9">
         <f t="shared" si="0"/>
-        <v>114876.35990534152</v>
-      </c>
-      <c r="S11" s="9">
+        <v>100145</v>
+      </c>
+      <c r="W11" s="10">
         <f t="shared" si="1"/>
-        <v>12.594228370284263</v>
-      </c>
-      <c r="T11" s="9">
-        <f t="shared" si="2"/>
-        <v>966.06000000000006</v>
-      </c>
-      <c r="U11" s="9">
-        <f t="shared" si="3"/>
-        <v>4436.72</v>
-      </c>
-      <c r="V11" s="9">
-        <f t="shared" si="4"/>
-        <v>5402.7800000000007</v>
-      </c>
-      <c r="W11" s="10">
-        <f t="shared" si="5"/>
-        <v>120291.73413371181</v>
-      </c>
-    </row>
-    <row r="12" spans="1:23" x14ac:dyDescent="0.3">
+        <v>215033.99423000001</v>
+      </c>
+    </row>
+    <row r="12" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A12" s="7" t="s">
         <v>74</v>
       </c>
       <c r="B12" s="8">
-        <f t="shared" si="6"/>
+        <f t="shared" si="2"/>
         <v>5365</v>
       </c>
       <c r="C12" s="8">
@@ -3833,32 +3767,28 @@
       <c r="Q12" s="8">
         <v>368464.72317224898</v>
       </c>
-      <c r="R12" s="9">
+      <c r="R12" s="12">
+        <v>115530.5</v>
+      </c>
+      <c r="S12" s="12">
+        <v>12.21167</v>
+      </c>
+      <c r="T12" s="12">
+        <v>7280</v>
+      </c>
+      <c r="U12" s="12">
+        <v>55966.5</v>
+      </c>
+      <c r="V12" s="9">
         <f t="shared" si="0"/>
-        <v>115530.46906962365</v>
-      </c>
-      <c r="S12" s="9">
+        <v>63246.5</v>
+      </c>
+      <c r="W12" s="10">
         <f t="shared" si="1"/>
-        <v>12.211670303203721</v>
-      </c>
-      <c r="T12" s="9">
-        <f t="shared" si="2"/>
-        <v>1502.2</v>
-      </c>
-      <c r="U12" s="9">
-        <f t="shared" si="3"/>
-        <v>17919.099999999999</v>
-      </c>
-      <c r="V12" s="9">
-        <f t="shared" si="4"/>
-        <v>19421.3</v>
-      </c>
-      <c r="W12" s="10">
-        <f t="shared" si="5"/>
-        <v>134963.98073992686</v>
-      </c>
-    </row>
-    <row r="13" spans="1:23" x14ac:dyDescent="0.3">
+        <v>178789.21166999999</v>
+      </c>
+    </row>
+    <row r="13" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A13" s="7" t="s">
         <v>75</v>
       </c>
@@ -3912,37 +3842,33 @@
         <f>$Q$12+20*$B$13</f>
         <v>1012244.723172249</v>
       </c>
-      <c r="R13" s="9">
+      <c r="R13" s="12">
+        <v>115530.5</v>
+      </c>
+      <c r="S13" s="12">
+        <v>25.08727</v>
+      </c>
+      <c r="T13" s="12">
+        <v>14160</v>
+      </c>
+      <c r="U13" s="12">
+        <v>106486.5</v>
+      </c>
+      <c r="V13" s="9">
         <f t="shared" si="0"/>
-        <v>115530.46906962365</v>
-      </c>
-      <c r="S13" s="9">
+        <v>120646.5</v>
+      </c>
+      <c r="W13" s="10">
         <f t="shared" si="1"/>
-        <v>25.08727030320372</v>
-      </c>
-      <c r="T13" s="9">
-        <f t="shared" si="2"/>
-        <v>17382.060000000001</v>
-      </c>
-      <c r="U13" s="9">
-        <f t="shared" si="3"/>
-        <v>108798.82</v>
-      </c>
-      <c r="V13" s="9">
-        <f t="shared" si="4"/>
-        <v>126180.88</v>
-      </c>
-      <c r="W13" s="10">
-        <f t="shared" si="5"/>
-        <v>241736.43633992688</v>
-      </c>
-    </row>
-    <row r="14" spans="1:23" x14ac:dyDescent="0.3">
+        <v>236202.08727000002</v>
+      </c>
+    </row>
+    <row r="14" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A14" s="7" t="s">
         <v>76</v>
       </c>
       <c r="B14" s="8">
-        <f t="shared" si="6"/>
+        <f t="shared" si="2"/>
         <v>5365</v>
       </c>
       <c r="C14" s="8">
@@ -3990,37 +3916,33 @@
       <c r="Q14" s="8">
         <v>387592.626526276</v>
       </c>
-      <c r="R14" s="9">
+      <c r="R14" s="12">
+        <v>114876.4</v>
+      </c>
+      <c r="S14" s="12">
+        <v>12.59423</v>
+      </c>
+      <c r="T14" s="12">
+        <v>14800</v>
+      </c>
+      <c r="U14" s="12">
+        <v>105356</v>
+      </c>
+      <c r="V14" s="9">
         <f t="shared" si="0"/>
-        <v>114876.35990534152</v>
-      </c>
-      <c r="S14" s="9">
+        <v>120156</v>
+      </c>
+      <c r="W14" s="10">
         <f t="shared" si="1"/>
-        <v>12.594228370284263</v>
-      </c>
-      <c r="T14" s="9">
-        <f t="shared" si="2"/>
-        <v>2897.1000000000004</v>
-      </c>
-      <c r="U14" s="9">
-        <f t="shared" si="3"/>
-        <v>13305.200000000003</v>
-      </c>
-      <c r="V14" s="9">
-        <f t="shared" si="4"/>
-        <v>16202.300000000003</v>
-      </c>
-      <c r="W14" s="10">
-        <f t="shared" si="5"/>
-        <v>131091.25413371183</v>
-      </c>
-    </row>
-    <row r="15" spans="1:23" x14ac:dyDescent="0.3">
+        <v>235044.99423000001</v>
+      </c>
+    </row>
+    <row r="15" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A15" s="7" t="s">
         <v>77</v>
       </c>
       <c r="B15" s="8">
-        <f t="shared" si="6"/>
+        <f t="shared" si="2"/>
         <v>5365</v>
       </c>
       <c r="C15" s="8">
@@ -4069,38 +3991,34 @@
         <f>$Q$12</f>
         <v>368464.72317224898</v>
       </c>
-      <c r="R15" s="9">
+      <c r="R15" s="12">
+        <v>115530.5</v>
+      </c>
+      <c r="S15" s="12">
+        <v>12.21167</v>
+      </c>
+      <c r="T15" s="12">
+        <v>14160</v>
+      </c>
+      <c r="U15" s="12">
+        <v>56966.5</v>
+      </c>
+      <c r="V15" s="9">
         <f t="shared" si="0"/>
-        <v>115530.46906962365</v>
-      </c>
-      <c r="S15" s="9">
+        <v>71126.5</v>
+      </c>
+      <c r="W15" s="10">
         <f t="shared" si="1"/>
-        <v>12.211670303203721</v>
-      </c>
-      <c r="T15" s="9">
-        <f t="shared" si="2"/>
-        <v>2897.1000000000004</v>
-      </c>
-      <c r="U15" s="9">
-        <f t="shared" si="3"/>
-        <v>18133.7</v>
-      </c>
-      <c r="V15" s="9">
-        <f t="shared" si="4"/>
-        <v>21030.800000000003</v>
-      </c>
-      <c r="W15" s="10">
-        <f t="shared" si="5"/>
-        <v>136573.48073992686</v>
-      </c>
-    </row>
-    <row r="27" spans="16:16" x14ac:dyDescent="0.3">
+        <v>186669.21166999999</v>
+      </c>
+    </row>
+    <row r="27" spans="16:16" x14ac:dyDescent="0.25">
       <c r="P27">
         <f>0.02/1000</f>
         <v>2.0000000000000002E-5</v>
       </c>
     </row>
-    <row r="42" spans="17:24" x14ac:dyDescent="0.3">
+    <row r="42" spans="17:24" x14ac:dyDescent="0.25">
       <c r="Q42" s="5" t="s">
         <v>54</v>
       </c>
@@ -4114,12 +4032,12 @@
         <v>55</v>
       </c>
     </row>
-    <row r="43" spans="17:24" x14ac:dyDescent="0.3">
+    <row r="43" spans="17:24" x14ac:dyDescent="0.25">
       <c r="R43" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="44" spans="17:24" x14ac:dyDescent="0.3">
+    <row r="44" spans="17:24" x14ac:dyDescent="0.25">
       <c r="Q44" t="s">
         <v>57</v>
       </c>
@@ -4139,7 +4057,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="45" spans="17:24" x14ac:dyDescent="0.3">
+    <row r="45" spans="17:24" x14ac:dyDescent="0.25">
       <c r="R45" t="s">
         <v>59</v>
       </c>
@@ -4150,7 +4068,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="46" spans="17:24" x14ac:dyDescent="0.3">
+    <row r="46" spans="17:24" x14ac:dyDescent="0.25">
       <c r="Q46" t="s">
         <v>62</v>
       </c>
@@ -4167,7 +4085,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="65" spans="1:25" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:25" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A65" s="6"/>
       <c r="B65" s="6"/>
       <c r="C65" s="6"/>
@@ -4213,7 +4131,7 @@
       <selection sqref="A1:U22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
@@ -5662,7 +5580,7 @@
       <selection sqref="A1:U22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
@@ -7111,12 +7029,12 @@
       <selection sqref="A1:U22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="19" max="19" width="16.88671875" customWidth="1"/>
+    <col min="19" max="19" width="16.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:21" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>25</v>
       </c>
@@ -7181,7 +7099,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="2" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:21" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>2018</v>
       </c>
@@ -7246,7 +7164,7 @@
         <v>-1406.1283124115794</v>
       </c>
     </row>
-    <row r="3" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:21" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>2019</v>
       </c>
@@ -7311,7 +7229,7 @@
         <v>-460.11664764689033</v>
       </c>
     </row>
-    <row r="4" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:21" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>2020</v>
       </c>
@@ -7376,7 +7294,7 @@
         <v>1029.6460228003475</v>
       </c>
     </row>
-    <row r="5" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:21" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>2021</v>
       </c>
@@ -7441,7 +7359,7 @@
         <v>3523.5700132144393</v>
       </c>
     </row>
-    <row r="6" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:21" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>2022</v>
       </c>
@@ -7506,7 +7424,7 @@
         <v>7801.2920480762359</v>
       </c>
     </row>
-    <row r="7" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:21" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>2023</v>
       </c>
@@ -7571,7 +7489,7 @@
         <v>15064.713468148853</v>
       </c>
     </row>
-    <row r="8" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:21" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>2024</v>
       </c>
@@ -7636,7 +7554,7 @@
         <v>27032.584081264151</v>
       </c>
     </row>
-    <row r="9" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:21" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>2025</v>
       </c>
@@ -7701,7 +7619,7 @@
         <v>45148.611713618346</v>
       </c>
     </row>
-    <row r="10" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:21" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>2026</v>
       </c>
@@ -7766,7 +7684,7 @@
         <v>68189.323906569727</v>
       </c>
     </row>
-    <row r="11" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:21" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>2027</v>
       </c>
@@ -7831,7 +7749,7 @@
         <v>88357.291589972039</v>
       </c>
     </row>
-    <row r="12" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:21" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>2028</v>
       </c>
@@ -7896,7 +7814,7 @@
         <v>94713.286097848322</v>
       </c>
     </row>
-    <row r="13" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:21" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>2029</v>
       </c>
@@ -7961,7 +7879,7 @@
         <v>88904.134606335574</v>
       </c>
     </row>
-    <row r="14" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:21" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>2030</v>
       </c>
@@ -8026,7 +7944,7 @@
         <v>80940.471215402416</v>
       </c>
     </row>
-    <row r="15" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:21" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>2031</v>
       </c>
@@ -8091,7 +8009,7 @@
         <v>73599.626422240937</v>
       </c>
     </row>
-    <row r="16" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:21" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>2032</v>
       </c>
@@ -8156,7 +8074,7 @@
         <v>66918.231218101311</v>
       </c>
     </row>
-    <row r="17" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:21" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>2033</v>
       </c>
@@ -8221,7 +8139,7 @@
         <v>60840.50106200423</v>
       </c>
     </row>
-    <row r="18" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:21" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>2034</v>
       </c>
@@ -8286,7 +8204,7 @@
         <v>55312.157969633328</v>
       </c>
     </row>
-    <row r="19" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:21" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>2035</v>
       </c>
@@ -8351,7 +8269,7 @@
         <v>50283.779972393932</v>
       </c>
     </row>
-    <row r="20" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:21" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>2036</v>
       </c>
@@ -8416,7 +8334,7 @@
         <v>45714.685553109754</v>
       </c>
     </row>
-    <row r="21" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:21" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>2037</v>
       </c>
@@ -8481,7 +8399,7 @@
         <v>41558.805048281589</v>
       </c>
     </row>
-    <row r="22" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:21" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A22">
         <v>2038</v>
       </c>
@@ -8546,7 +8464,7 @@
         <v>37780.731862074172</v>
       </c>
     </row>
-    <row r="46" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="46" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
@@ -8564,7 +8482,7 @@
       <selection sqref="A1:U22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
@@ -10013,7 +9931,7 @@
       <selection sqref="A1:U22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
@@ -11462,7 +11380,7 @@
       <selection activeCell="Q43" sqref="Q43"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
@@ -12911,7 +12829,7 @@
       <selection sqref="A1:U22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
@@ -14360,7 +14278,7 @@
       <selection activeCell="O39" sqref="O39"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
@@ -15807,26 +15725,26 @@
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="L2" sqref="L2"/>
+      <selection pane="topRight" activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="30.88671875" customWidth="1"/>
+    <col min="1" max="1" width="30.85546875" customWidth="1"/>
     <col min="2" max="2" width="28" customWidth="1"/>
     <col min="3" max="3" width="18" customWidth="1"/>
-    <col min="4" max="4" width="20.6640625" customWidth="1"/>
-    <col min="5" max="5" width="19.33203125" customWidth="1"/>
-    <col min="6" max="6" width="34.5546875" customWidth="1"/>
-    <col min="7" max="7" width="22.6640625" customWidth="1"/>
+    <col min="4" max="4" width="20.7109375" customWidth="1"/>
+    <col min="5" max="5" width="19.28515625" customWidth="1"/>
+    <col min="6" max="6" width="34.5703125" customWidth="1"/>
+    <col min="7" max="7" width="22.7109375" customWidth="1"/>
     <col min="8" max="8" width="25" customWidth="1"/>
-    <col min="9" max="9" width="17.33203125" customWidth="1"/>
+    <col min="9" max="9" width="17.28515625" customWidth="1"/>
     <col min="10" max="10" width="16" customWidth="1"/>
-    <col min="11" max="11" width="16.88671875" customWidth="1"/>
-    <col min="12" max="12" width="12.5546875" customWidth="1"/>
-    <col min="13" max="13" width="15.33203125" customWidth="1"/>
-    <col min="14" max="14" width="16.44140625" customWidth="1"/>
-    <col min="15" max="15" width="25.6640625" customWidth="1"/>
+    <col min="11" max="11" width="16.85546875" customWidth="1"/>
+    <col min="12" max="12" width="12.5703125" customWidth="1"/>
+    <col min="13" max="13" width="15.28515625" customWidth="1"/>
+    <col min="14" max="14" width="16.42578125" customWidth="1"/>
+    <col min="15" max="15" width="25.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:15" x14ac:dyDescent="0.3">
@@ -15885,55 +15803,55 @@
       </c>
       <c r="C2">
         <f>CAPEX!$W3</f>
-        <v>153117.87443632298</v>
+        <v>341809.22911888885</v>
       </c>
       <c r="D2">
         <f>CAPEX!$W4</f>
-        <v>160728.88879802052</v>
+        <v>215018.54792333333</v>
       </c>
       <c r="E2">
         <f>CAPEX!$W5</f>
-        <v>96805.798673873811</v>
+        <v>143587.08878666669</v>
       </c>
       <c r="F2">
         <f>CAPEX!$W6</f>
-        <v>207428.10534054047</v>
+        <v>156832.13545333332</v>
       </c>
       <c r="G2">
         <f>CAPEX!$W7</f>
-        <v>232617.20879802053</v>
+        <v>227169.58125666663</v>
       </c>
       <c r="H2">
         <f>CAPEX!$W8</f>
-        <v>167172.91443632299</v>
+        <v>347869.80689666665</v>
       </c>
       <c r="I2">
         <f>CAPEX!$W9</f>
-        <v>164913.5887980205</v>
+        <v>221159.28125666664</v>
       </c>
       <c r="J2">
         <f>CAPEX!$W10</f>
-        <v>96913.098673873814</v>
+        <v>146300.63545333332</v>
       </c>
       <c r="K2">
         <f>CAPEX!$W11</f>
-        <v>120291.73413371181</v>
+        <v>215033.99423000001</v>
       </c>
       <c r="L2">
         <f>CAPEX!$W12</f>
-        <v>134963.98073992686</v>
+        <v>178789.21166999999</v>
       </c>
       <c r="M2">
         <f>CAPEX!$W13</f>
-        <v>241736.43633992688</v>
+        <v>236202.08727000002</v>
       </c>
       <c r="N2">
         <f>CAPEX!$W14</f>
-        <v>131091.25413371183</v>
+        <v>235044.99423000001</v>
       </c>
       <c r="O2">
         <f>CAPEX!$W15</f>
-        <v>136573.48073992686</v>
+        <v>186669.21166999999</v>
       </c>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.3">
@@ -15948,7 +15866,7 @@
       </c>
       <c r="D3">
         <f>D2-C2</f>
-        <v>7611.0143616975402</v>
+        <v>-126790.68119555552</v>
       </c>
       <c r="E3">
         <v>0</v>
@@ -15958,15 +15876,15 @@
       </c>
       <c r="G3">
         <f>G2-C2</f>
-        <v>79499.334361697547</v>
+        <v>-114639.64786222222</v>
       </c>
       <c r="H3">
         <f>H2-C2</f>
-        <v>14055.040000000008</v>
+        <v>6060.5777777777985</v>
       </c>
       <c r="I3">
         <f>D3+(I2-D2)</f>
-        <v>11795.714361697523</v>
+        <v>-120649.94786222221</v>
       </c>
       <c r="J3">
         <v>0</v>
@@ -16008,14 +15926,14 @@
       </c>
       <c r="G4">
         <f>G2-D2</f>
-        <v>71888.320000000007</v>
+        <v>12151.033333333296</v>
       </c>
       <c r="H4">
         <v>0</v>
       </c>
       <c r="I4">
         <f>I2-D2</f>
-        <v>4184.6999999999825</v>
+        <v>6140.7333333333081</v>
       </c>
       <c r="J4">
         <v>0</v>
@@ -16054,7 +15972,7 @@
       </c>
       <c r="F5">
         <f>F2-E2</f>
-        <v>110622.30666666666</v>
+        <v>13245.046666666633</v>
       </c>
       <c r="G5">
         <v>0</v>
@@ -16067,7 +15985,7 @@
       </c>
       <c r="J5">
         <f>J2-E2</f>
-        <v>107.30000000000291</v>
+        <v>2713.5466666666325</v>
       </c>
       <c r="K5">
         <v>0</v>
@@ -16200,14 +16118,14 @@
       </c>
       <c r="G8">
         <f>G2-H2</f>
-        <v>65444.294361697539</v>
+        <v>-120700.22564000002</v>
       </c>
       <c r="H8">
         <v>0</v>
       </c>
       <c r="I8">
         <f>I2-H2</f>
-        <v>-2259.3256383024855</v>
+        <v>-126710.52564000001</v>
       </c>
       <c r="J8">
         <v>0</v>
@@ -16249,7 +16167,7 @@
       </c>
       <c r="G9">
         <f>G2-I2</f>
-        <v>67703.620000000024</v>
+        <v>6010.2999999999884</v>
       </c>
       <c r="H9">
         <v>0</v>
@@ -16294,7 +16212,7 @@
       </c>
       <c r="F10">
         <f>F2-J2</f>
-        <v>110515.00666666665</v>
+        <v>10531.5</v>
       </c>
       <c r="G10">
         <v>0</v>
@@ -16360,19 +16278,19 @@
       </c>
       <c r="L11">
         <f>L2-K2</f>
-        <v>14672.246606215049</v>
+        <v>-36244.782560000021</v>
       </c>
       <c r="M11">
         <f>M2-K2</f>
-        <v>121444.70220621506</v>
+        <v>21168.093040000007</v>
       </c>
       <c r="N11">
         <f>N2-K2</f>
-        <v>10799.520000000019</v>
+        <v>20011</v>
       </c>
       <c r="O11">
         <f>L11+(O2-L2)</f>
-        <v>16281.746606215049</v>
+        <v>-28364.782560000021</v>
       </c>
     </row>
     <row r="12" spans="1:15" x14ac:dyDescent="0.3">
@@ -16414,14 +16332,14 @@
       </c>
       <c r="M12">
         <f>M2-L2</f>
-        <v>106772.45560000002</v>
+        <v>57412.875600000028</v>
       </c>
       <c r="N12">
         <v>0</v>
       </c>
       <c r="O12">
         <f>O2-L2</f>
-        <v>1609.5</v>
+        <v>7880</v>
       </c>
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.3">
@@ -16510,14 +16428,14 @@
       </c>
       <c r="M14">
         <f>M2-N2</f>
-        <v>110645.18220621505</v>
+        <v>1157.093040000007</v>
       </c>
       <c r="N14">
         <v>0</v>
       </c>
       <c r="O14">
         <f>O2-N2</f>
-        <v>5482.2266062150302</v>
+        <v>-48375.782560000021</v>
       </c>
     </row>
     <row r="15" spans="1:15" x14ac:dyDescent="0.3">
@@ -16559,7 +16477,7 @@
       </c>
       <c r="M15">
         <f>M2-O2</f>
-        <v>105162.95560000002</v>
+        <v>49532.875600000028</v>
       </c>
       <c r="N15">
         <v>0</v>
@@ -16582,14 +16500,14 @@
   <dimension ref="A1:C15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A21" sqref="A21"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="27.6640625" customWidth="1"/>
-    <col min="2" max="2" width="39.88671875" customWidth="1"/>
-    <col min="3" max="3" width="15.109375" customWidth="1"/>
+    <col min="1" max="1" width="27.7109375" customWidth="1"/>
+    <col min="2" max="2" width="39.85546875" customWidth="1"/>
+    <col min="3" max="3" width="15.140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.3">
@@ -16608,7 +16526,8 @@
         <v>24</v>
       </c>
       <c r="B2">
-        <v>2500</v>
+        <f>AVERAGE(B3:B15)</f>
+        <v>11239.427296319658</v>
       </c>
       <c r="C2">
         <v>3.6</v>
@@ -16620,7 +16539,7 @@
       </c>
       <c r="B3">
         <f>0.1*(CAPEX!T3+CAPEX!U3)+0.01*(CAPEX!R3+CAPEX!S3)</f>
-        <v>2139.68314436323</v>
+        <v>21008.816291188887</v>
       </c>
       <c r="C3">
         <v>7.2</v>
@@ -16632,7 +16551,7 @@
       </c>
       <c r="B4">
         <f>0.1*(CAPEX!T4+CAPEX!U4)+0.01*(CAPEX!R4+CAPEX!S4)</f>
-        <v>2901.3268879802054</v>
+        <v>8330.290479233332</v>
       </c>
       <c r="C4">
         <v>9.6</v>
@@ -16644,7 +16563,7 @@
       </c>
       <c r="B5">
         <f>0.1*(CAPEX!T5+CAPEX!U5)+0.01*(CAPEX!R5+CAPEX!S5)</f>
-        <v>2580.7769867387378</v>
+        <v>7258.905687866667</v>
       </c>
       <c r="C5">
         <v>9.6</v>
@@ -16656,7 +16575,7 @@
       </c>
       <c r="B6">
         <f>0.1*(CAPEX!T6+CAPEX!U6)+0.01*(CAPEX!R6+CAPEX!S6)</f>
-        <v>13643.007653405404</v>
+        <v>8583.4103545333346</v>
       </c>
       <c r="C6">
         <v>12</v>
@@ -16668,7 +16587,7 @@
       </c>
       <c r="B7">
         <f>0.1*(CAPEX!T7+CAPEX!U7)+0.01*(CAPEX!R7+CAPEX!S7)</f>
-        <v>10090.158887980206</v>
+        <v>9545.3938125666664</v>
       </c>
       <c r="C7">
         <v>12</v>
@@ -16680,7 +16599,7 @@
       </c>
       <c r="B8">
         <f>0.1*(CAPEX!T8+CAPEX!U8)+0.01*(CAPEX!R8+CAPEX!S8)</f>
-        <v>3545.1871443632299</v>
+        <v>21614.874068966667</v>
       </c>
       <c r="C8">
         <v>12</v>
@@ -16692,7 +16611,7 @@
       </c>
       <c r="B9">
         <f>0.1*(CAPEX!T9+CAPEX!U9)+0.01*(CAPEX!R9+CAPEX!S9)</f>
-        <v>3319.7968879802052</v>
+        <v>8944.3638125666657</v>
       </c>
       <c r="C9">
         <v>12</v>
@@ -16704,7 +16623,7 @@
       </c>
       <c r="B10">
         <f>0.1*(CAPEX!T10+CAPEX!U10)+0.01*(CAPEX!R10+CAPEX!S10)</f>
-        <v>2591.5069867387383</v>
+        <v>7530.2603545333332</v>
       </c>
       <c r="C10">
         <v>12</v>
@@ -16716,7 +16635,7 @@
       </c>
       <c r="B11">
         <f>0.1*(CAPEX!T11+CAPEX!U11)+0.01*(CAPEX!R11+CAPEX!S11)</f>
-        <v>1689.1675413371181</v>
+        <v>11163.3899423</v>
       </c>
       <c r="C11">
         <v>7.2</v>
@@ -16728,7 +16647,7 @@
       </c>
       <c r="B12">
         <f>0.1*(CAPEX!T12+CAPEX!U12)+0.01*(CAPEX!R12+CAPEX!S12)</f>
-        <v>3097.556807399269</v>
+        <v>7480.0771167000003</v>
       </c>
       <c r="C12">
         <v>9.6</v>
@@ -16740,7 +16659,7 @@
       </c>
       <c r="B13">
         <f>0.1*(CAPEX!T13+CAPEX!U13)+0.01*(CAPEX!R13+CAPEX!S13)</f>
-        <v>13773.64356339927</v>
+        <v>13220.205872700002</v>
       </c>
       <c r="C13">
         <v>12</v>
@@ -16752,7 +16671,7 @@
       </c>
       <c r="B14">
         <f>0.1*(CAPEX!T14+CAPEX!U14)+0.01*(CAPEX!R14+CAPEX!S14)</f>
-        <v>2769.1195413371188</v>
+        <v>13164.489942300001</v>
       </c>
       <c r="C14">
         <v>12</v>
@@ -16764,7 +16683,7 @@
       </c>
       <c r="B15">
         <f>0.1*(CAPEX!T15+CAPEX!U15)+0.01*(CAPEX!R15+CAPEX!S15)</f>
-        <v>3258.5068073992688</v>
+        <v>8268.0771167000003</v>
       </c>
       <c r="C15">
         <v>12</v>
@@ -16788,17 +16707,17 @@
       <selection activeCell="R17" sqref="R17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="16.6640625" customWidth="1"/>
-    <col min="3" max="3" width="15.109375" customWidth="1"/>
-    <col min="4" max="4" width="15.5546875" customWidth="1"/>
-    <col min="5" max="5" width="19.33203125" customWidth="1"/>
-    <col min="6" max="6" width="20.44140625" customWidth="1"/>
-    <col min="7" max="7" width="23.5546875" customWidth="1"/>
+    <col min="2" max="2" width="16.7109375" customWidth="1"/>
+    <col min="3" max="3" width="15.140625" customWidth="1"/>
+    <col min="4" max="4" width="15.5703125" customWidth="1"/>
+    <col min="5" max="5" width="19.28515625" customWidth="1"/>
+    <col min="6" max="6" width="20.42578125" customWidth="1"/>
+    <col min="7" max="7" width="23.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:34" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:34" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>25</v>
       </c>
@@ -16878,7 +16797,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="2" spans="1:34" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:34" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A2" s="1">
         <v>2018</v>
       </c>
@@ -16926,31 +16845,31 @@
       </c>
       <c r="U2">
         <f>OPEX!$B$3</f>
-        <v>2139.68314436323</v>
+        <v>21008.816291188887</v>
       </c>
       <c r="V2">
         <f>O2-U2</f>
-        <v>-1448.4831443632299</v>
+        <v>-20317.616291188886</v>
       </c>
       <c r="W2">
         <f>P2-U2</f>
-        <v>-1448.4831443632299</v>
+        <v>-20317.616291188886</v>
       </c>
       <c r="X2">
         <f t="shared" ref="X2:X22" si="1">Q2-U2</f>
-        <v>-1448.4831443632299</v>
+        <v>-20317.616291188886</v>
       </c>
       <c r="Y2">
         <f>R2-$U2</f>
-        <v>-1520.4831443632299</v>
+        <v>-20389.616291188886</v>
       </c>
       <c r="Z2">
         <f>S2-$U2</f>
-        <v>-1520.4831443632299</v>
+        <v>-20389.616291188886</v>
       </c>
       <c r="AA2">
         <f>T2-$U2</f>
-        <v>-1520.4831443632299</v>
+        <v>-20389.616291188886</v>
       </c>
       <c r="AB2">
         <f>1/POWER(1+$L$25,N2-2018)</f>
@@ -16958,30 +16877,30 @@
       </c>
       <c r="AC2">
         <f>V2*AB2</f>
-        <v>-1448.4831443632299</v>
+        <v>-20317.616291188886</v>
       </c>
       <c r="AD2">
         <f>W2*AB2</f>
-        <v>-1448.4831443632299</v>
+        <v>-20317.616291188886</v>
       </c>
       <c r="AE2">
         <f>X2*AB2</f>
-        <v>-1448.4831443632299</v>
+        <v>-20317.616291188886</v>
       </c>
       <c r="AF2">
         <f>Y2*$AB2</f>
-        <v>-1520.4831443632299</v>
+        <v>-20389.616291188886</v>
       </c>
       <c r="AG2">
         <f>Z2*$AB2</f>
-        <v>-1520.4831443632299</v>
+        <v>-20389.616291188886</v>
       </c>
       <c r="AH2">
         <f>AA2*$AB2</f>
-        <v>-1520.4831443632299</v>
-      </c>
-    </row>
-    <row r="3" spans="1:34" x14ac:dyDescent="0.3">
+        <v>-20389.616291188886</v>
+      </c>
+    </row>
+    <row r="3" spans="1:34" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A3" s="1">
         <v>2019</v>
       </c>
@@ -17028,31 +16947,31 @@
       </c>
       <c r="U3">
         <f>OPEX!$B$3</f>
-        <v>2139.68314436323</v>
+        <v>21008.816291188887</v>
       </c>
       <c r="V3">
         <f t="shared" ref="V3:V22" si="8">O3-U3</f>
-        <v>-1218.0831443632301</v>
+        <v>-20087.216291188888</v>
       </c>
       <c r="W3">
         <f t="shared" ref="W3:W22" si="9">P3-U3</f>
-        <v>-1189.2831443632299</v>
+        <v>-20058.416291188885</v>
       </c>
       <c r="X3">
         <f t="shared" si="1"/>
-        <v>-850.88314436323003</v>
+        <v>-19720.016291188887</v>
       </c>
       <c r="Y3">
         <f t="shared" ref="Y3:Y22" si="10">R3-$U3</f>
-        <v>-1311.68314436323</v>
+        <v>-20180.816291188887</v>
       </c>
       <c r="Z3">
         <f t="shared" ref="Z3:Z22" si="11">S3-$U3</f>
-        <v>-1290.0831443632301</v>
+        <v>-20159.216291188888</v>
       </c>
       <c r="AA3">
         <f t="shared" ref="AA3:AA22" si="12">T3-$U3</f>
-        <v>-980.48314436322994</v>
+        <v>-19849.616291188886</v>
       </c>
       <c r="AB3">
         <f t="shared" ref="AB3:AB22" si="13">1/POWER(1+$L$25,N3-2018)</f>
@@ -17060,30 +16979,30 @@
       </c>
       <c r="AC3">
         <f t="shared" ref="AC3:AC22" si="14">V3*AB3</f>
-        <v>-1107.3483130574818</v>
+        <v>-18261.105719262625</v>
       </c>
       <c r="AD3">
         <f t="shared" ref="AD3:AD22" si="15">W3*AB3</f>
-        <v>-1081.1664948756636</v>
+        <v>-18234.923901080805</v>
       </c>
       <c r="AE3">
         <f t="shared" ref="AE3:AE22" si="16">X3*AB3</f>
-        <v>-773.53013123929998</v>
+        <v>-17927.287537444441</v>
       </c>
       <c r="AF3">
         <f t="shared" ref="AF3:AF22" si="17">Y3*$AB3</f>
-        <v>-1192.4392221483909</v>
+        <v>-18346.196628353533</v>
       </c>
       <c r="AG3">
         <f t="shared" ref="AG3:AG22" si="18">Z3*$AB3</f>
-        <v>-1172.8028585120273</v>
+        <v>-18326.560264717169</v>
       </c>
       <c r="AH3">
         <f t="shared" ref="AH3:AH22" si="19">AA3*$AB3</f>
-        <v>-891.34831305748173</v>
-      </c>
-    </row>
-    <row r="4" spans="1:34" x14ac:dyDescent="0.3">
+        <v>-18045.105719262621</v>
+      </c>
+    </row>
+    <row r="4" spans="1:34" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A4" s="1">
         <v>2020</v>
       </c>
@@ -17130,31 +17049,31 @@
       </c>
       <c r="U4">
         <f>OPEX!$B$3</f>
-        <v>2139.68314436323</v>
+        <v>21008.816291188887</v>
       </c>
       <c r="V4">
         <f t="shared" si="8"/>
-        <v>-901.28314436322989</v>
+        <v>-19770.416291188885</v>
       </c>
       <c r="W4">
         <f t="shared" si="9"/>
-        <v>-822.08314436322985</v>
+        <v>-19691.216291188888</v>
       </c>
       <c r="X4">
         <f t="shared" si="1"/>
-        <v>322.71685563677011</v>
+        <v>-18546.416291188885</v>
       </c>
       <c r="Y4">
         <f t="shared" si="10"/>
-        <v>-1030.88314436323</v>
+        <v>-19900.016291188887</v>
       </c>
       <c r="Z4">
         <f t="shared" si="11"/>
-        <v>-958.88314436323003</v>
+        <v>-19828.016291188887</v>
       </c>
       <c r="AA4">
         <f t="shared" si="12"/>
-        <v>70.716855636770106</v>
+        <v>-18798.416291188885</v>
       </c>
       <c r="AB4">
         <f t="shared" si="13"/>
@@ -17162,30 +17081,30 @@
       </c>
       <c r="AC4">
         <f t="shared" si="14"/>
-        <v>-744.86210277952875</v>
+        <v>-16339.187017511475</v>
       </c>
       <c r="AD4">
         <f t="shared" si="15"/>
-        <v>-679.40755732498326</v>
+        <v>-16273.73247205693</v>
       </c>
       <c r="AE4">
         <f t="shared" si="16"/>
-        <v>266.70814515435541</v>
+        <v>-15327.616769577589</v>
       </c>
       <c r="AF4">
         <f t="shared" si="17"/>
-        <v>-851.9695407960578</v>
+        <v>-16446.294455528005</v>
       </c>
       <c r="AG4">
         <f t="shared" si="18"/>
-        <v>-792.46540856465288</v>
+        <v>-16386.790323296598</v>
       </c>
       <c r="AH4">
         <f t="shared" si="19"/>
-        <v>58.443682344438095</v>
-      </c>
-    </row>
-    <row r="5" spans="1:34" x14ac:dyDescent="0.3">
+        <v>-15535.881232387506</v>
+      </c>
+    </row>
+    <row r="5" spans="1:34" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A5" s="1">
         <v>2021</v>
       </c>
@@ -17239,31 +17158,31 @@
       </c>
       <c r="U5">
         <f>OPEX!$B$3</f>
-        <v>2139.68314436323</v>
+        <v>21008.816291188887</v>
       </c>
       <c r="V5">
         <f t="shared" si="8"/>
-        <v>-462.08314436322985</v>
+        <v>-19331.216291188888</v>
       </c>
       <c r="W5">
         <f t="shared" si="9"/>
-        <v>-289.28314436322989</v>
+        <v>-19158.416291188885</v>
       </c>
       <c r="X5">
         <f t="shared" si="1"/>
-        <v>2619.5168556367698</v>
+        <v>-16249.616291188886</v>
       </c>
       <c r="Y5">
         <f t="shared" si="10"/>
-        <v>-634.88314436323003</v>
+        <v>-19504.016291188887</v>
       </c>
       <c r="Z5">
         <f t="shared" si="11"/>
-        <v>-476.48314436322994</v>
+        <v>-19345.616291188886</v>
       </c>
       <c r="AA5">
         <f t="shared" si="12"/>
-        <v>2137.1168556367702</v>
+        <v>-16732.016291188887</v>
       </c>
       <c r="AB5">
         <f t="shared" si="13"/>
@@ -17271,30 +17190,30 @@
       </c>
       <c r="AC5">
         <f t="shared" si="14"/>
-        <v>-347.16990560723497</v>
+        <v>-14523.828918999912</v>
       </c>
       <c r="AD5">
         <f t="shared" si="15"/>
-        <v>-217.34270801144237</v>
+        <v>-14394.001721404116</v>
       </c>
       <c r="AE5">
         <f t="shared" si="16"/>
-        <v>1968.0817848510662</v>
+        <v>-12208.577228541608</v>
       </c>
       <c r="AF5">
         <f t="shared" si="17"/>
-        <v>-476.99710320302768</v>
+        <v>-14653.656116595705</v>
       </c>
       <c r="AG5">
         <f t="shared" si="18"/>
-        <v>-357.98883874021772</v>
+        <v>-14534.647852132894</v>
       </c>
       <c r="AH5">
         <f t="shared" si="19"/>
-        <v>1605.6475248961453</v>
-      </c>
-    </row>
-    <row r="6" spans="1:34" x14ac:dyDescent="0.3">
+        <v>-12571.011488496531</v>
+      </c>
+    </row>
+    <row r="6" spans="1:34" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A6" s="1">
         <v>2022</v>
       </c>
@@ -17348,31 +17267,31 @@
       </c>
       <c r="U6">
         <f>OPEX!$B$3</f>
-        <v>2139.68314436323</v>
+        <v>21008.816291188887</v>
       </c>
       <c r="V6">
         <f t="shared" si="8"/>
-        <v>149.91685563676992</v>
+        <v>-18719.216291188888</v>
       </c>
       <c r="W6">
         <f t="shared" si="9"/>
-        <v>473.91685563676992</v>
+        <v>-18395.216291188888</v>
       </c>
       <c r="X6">
         <f t="shared" si="1"/>
-        <v>7105.1168556367711</v>
+        <v>-11764.016291188886</v>
       </c>
       <c r="Y6">
         <f t="shared" si="10"/>
-        <v>-80.483144363229712</v>
+        <v>-18949.616291188886</v>
       </c>
       <c r="Z6">
         <f t="shared" si="11"/>
-        <v>207.51685563677029</v>
+        <v>-18661.616291188886</v>
       </c>
       <c r="AA6">
         <f t="shared" si="12"/>
-        <v>6176.31685563677</v>
+        <v>-12692.816291188887</v>
       </c>
       <c r="AB6">
         <f t="shared" si="13"/>
@@ -17380,30 +17299,30 @@
       </c>
       <c r="AC6">
         <f t="shared" si="14"/>
-        <v>102.39522958593668</v>
+        <v>-12785.476600771042</v>
       </c>
       <c r="AD6">
         <f t="shared" si="15"/>
-        <v>323.69158912421955</v>
+        <v>-12564.18024123276</v>
       </c>
       <c r="AE6">
         <f t="shared" si="16"/>
-        <v>4852.8904143410764</v>
+        <v>-8034.9814160159021</v>
       </c>
       <c r="AF6">
         <f t="shared" si="17"/>
-        <v>-54.971070530175325</v>
+        <v>-12942.842900887154</v>
       </c>
       <c r="AG6">
         <f t="shared" si="18"/>
-        <v>141.736804614965</v>
+        <v>-12746.135025742013</v>
       </c>
       <c r="AH6">
         <f t="shared" si="19"/>
-        <v>4218.5075169979973</v>
-      </c>
-    </row>
-    <row r="7" spans="1:34" x14ac:dyDescent="0.3">
+        <v>-8669.3643133589812</v>
+      </c>
+    </row>
+    <row r="7" spans="1:34" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A7" s="1">
         <v>2023</v>
       </c>
@@ -17457,31 +17376,31 @@
       </c>
       <c r="U7">
         <f>OPEX!$B$3</f>
-        <v>2139.68314436323</v>
+        <v>21008.816291188887</v>
       </c>
       <c r="V7">
         <f t="shared" si="8"/>
-        <v>992.31685563677001</v>
+        <v>-17876.816291188887</v>
       </c>
       <c r="W7">
         <f t="shared" si="9"/>
-        <v>1561.1168556367702</v>
+        <v>-17308.016291188887</v>
       </c>
       <c r="X7">
         <f t="shared" si="1"/>
-        <v>15665.916855636773</v>
+        <v>-3203.2162911888845</v>
       </c>
       <c r="Y7">
         <f t="shared" si="10"/>
-        <v>675.51685563677029</v>
+        <v>-18193.616291188886</v>
       </c>
       <c r="Z7">
         <f t="shared" si="11"/>
-        <v>1186.7168556367701</v>
+        <v>-17682.416291188885</v>
       </c>
       <c r="AA7">
         <f t="shared" si="12"/>
-        <v>13880.316855636771</v>
+        <v>-4988.8162911888867</v>
       </c>
       <c r="AB7">
         <f t="shared" si="13"/>
@@ -17489,30 +17408,30 @@
       </c>
       <c r="AC7">
         <f t="shared" si="14"/>
-        <v>616.1506948958837</v>
+        <v>-11100.096423610459</v>
       </c>
       <c r="AD7">
         <f t="shared" si="15"/>
-        <v>969.33074345193108</v>
+        <v>-10746.916375054412</v>
       </c>
       <c r="AE7">
         <f t="shared" si="16"/>
-        <v>9727.3018209367019</v>
+        <v>-1988.9452975696415</v>
       </c>
       <c r="AF7">
         <f t="shared" si="17"/>
-        <v>419.44281975074358</v>
+        <v>-11296.804298755598</v>
       </c>
       <c r="AG7">
         <f t="shared" si="18"/>
-        <v>736.85780009858343</v>
+        <v>-10979.389318407759</v>
       </c>
       <c r="AH7">
         <f t="shared" si="19"/>
-        <v>8618.5847064822738</v>
-      </c>
-    </row>
-    <row r="8" spans="1:34" x14ac:dyDescent="0.3">
+        <v>-3097.6624120240699</v>
+      </c>
+    </row>
+    <row r="8" spans="1:34" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A8" s="1">
         <v>2024</v>
       </c>
@@ -17566,31 +17485,31 @@
       </c>
       <c r="U8">
         <f>OPEX!$B$3</f>
-        <v>2139.68314436323</v>
+        <v>21008.816291188887</v>
       </c>
       <c r="V8">
         <f t="shared" si="8"/>
-        <v>2137.1168556367702</v>
+        <v>-16732.016291188887</v>
       </c>
       <c r="W8">
         <f t="shared" si="9"/>
-        <v>3094.7168556367706</v>
+        <v>-15774.416291188885</v>
       </c>
       <c r="X8">
         <f t="shared" si="1"/>
-        <v>31412.316855636771</v>
+        <v>12543.183708811113</v>
       </c>
       <c r="Y8">
         <f t="shared" si="10"/>
-        <v>1705.1168556367702</v>
+        <v>-17164.016291188887</v>
       </c>
       <c r="Z8">
         <f t="shared" si="11"/>
-        <v>2569.1168556367702</v>
+        <v>-16300.016291188887</v>
       </c>
       <c r="AA8">
         <f t="shared" si="12"/>
-        <v>28057.11685563677</v>
+        <v>9187.9837088111126</v>
       </c>
       <c r="AB8">
         <f t="shared" si="13"/>
@@ -17598,30 +17517,30 @@
       </c>
       <c r="AC8">
         <f t="shared" si="14"/>
-        <v>1206.3467504854584</v>
+        <v>-9444.7869936112165</v>
       </c>
       <c r="AD8">
         <f t="shared" si="15"/>
-        <v>1746.8869859049557</v>
+        <v>-8904.246758191719</v>
       </c>
       <c r="AE8">
         <f t="shared" si="16"/>
-        <v>17731.433947595797</v>
+        <v>7080.3002034991223</v>
       </c>
       <c r="AF8">
         <f t="shared" si="17"/>
-        <v>962.49401270222677</v>
+        <v>-9688.639731394449</v>
       </c>
       <c r="AG8">
         <f t="shared" si="18"/>
-        <v>1450.1994882686902</v>
+        <v>-9200.9342558279859</v>
       </c>
       <c r="AH8">
         <f t="shared" si="19"/>
-        <v>15837.511017479364</v>
-      </c>
-    </row>
-    <row r="9" spans="1:34" x14ac:dyDescent="0.3">
+        <v>5186.3772733826881</v>
+      </c>
+    </row>
+    <row r="9" spans="1:34" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A9" s="1">
         <v>2025</v>
       </c>
@@ -17674,31 +17593,31 @@
       </c>
       <c r="U9">
         <f>OPEX!$B$3</f>
-        <v>2139.68314436323</v>
+        <v>21008.816291188887</v>
       </c>
       <c r="V9">
         <f t="shared" si="8"/>
-        <v>3713.9168556367704</v>
+        <v>-15155.216291188886</v>
       </c>
       <c r="W9">
         <f t="shared" si="9"/>
-        <v>5254.7168556367706</v>
+        <v>-13614.416291188885</v>
       </c>
       <c r="X9">
         <f t="shared" si="1"/>
-        <v>58145.916855636766</v>
+        <v>39276.783708811112</v>
       </c>
       <c r="Y9">
         <f t="shared" si="10"/>
-        <v>3123.5168556367698</v>
+        <v>-15745.616291188886</v>
       </c>
       <c r="Z9">
         <f t="shared" si="11"/>
-        <v>4513.1168556367702</v>
+        <v>-14356.016291188887</v>
       </c>
       <c r="AA9">
         <f t="shared" si="12"/>
-        <v>52112.316855636767</v>
+        <v>33243.183708811113</v>
       </c>
       <c r="AB9">
         <f t="shared" si="13"/>
@@ -17706,30 +17625,30 @@
       </c>
       <c r="AC9">
         <f t="shared" si="14"/>
-        <v>1905.8265849038673</v>
+        <v>-7777.0222733658347</v>
       </c>
       <c r="AD9">
         <f t="shared" si="15"/>
-        <v>2696.50061347374</v>
+        <v>-6986.3482447959623</v>
       </c>
       <c r="AE9">
         <f t="shared" si="16"/>
-        <v>29838.04927643768</v>
+        <v>20155.200418167977</v>
       </c>
       <c r="AF9">
         <f t="shared" si="17"/>
-        <v>1602.8580319004579</v>
+        <v>-8079.9908263692441</v>
       </c>
       <c r="AG9">
         <f t="shared" si="18"/>
-        <v>2315.942552993848</v>
+        <v>-7366.9063052758547</v>
       </c>
       <c r="AH9">
         <f t="shared" si="19"/>
-        <v>26741.858454280889</v>
-      </c>
-    </row>
-    <row r="10" spans="1:34" x14ac:dyDescent="0.3">
+        <v>17059.009596011187</v>
+      </c>
+    </row>
+    <row r="10" spans="1:34" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A10" s="1">
         <v>2026</v>
       </c>
@@ -17782,31 +17701,31 @@
       </c>
       <c r="U10">
         <f>OPEX!$B$3</f>
-        <v>2139.68314436323</v>
+        <v>21008.816291188887</v>
       </c>
       <c r="V10">
         <f t="shared" si="8"/>
-        <v>5845.1168556367702</v>
+        <v>-13024.016291188887</v>
       </c>
       <c r="W10">
         <f t="shared" si="9"/>
-        <v>8271.5168556367717</v>
+        <v>-10597.616291188886</v>
       </c>
       <c r="X10">
         <f t="shared" si="1"/>
-        <v>96932.316855636775</v>
+        <v>78063.183708811121</v>
       </c>
       <c r="Y10">
         <f t="shared" si="10"/>
-        <v>5045.9168556367704</v>
+        <v>-13823.216291188886</v>
       </c>
       <c r="Z10">
         <f t="shared" si="11"/>
-        <v>7227.5168556367707</v>
+        <v>-11641.616291188886</v>
       </c>
       <c r="AA10">
         <f t="shared" si="12"/>
-        <v>87025.116855636777</v>
+        <v>68155.983708811109</v>
       </c>
       <c r="AB10">
         <f t="shared" si="13"/>
@@ -17814,30 +17733,30 @@
       </c>
       <c r="AC10">
         <f t="shared" si="14"/>
-        <v>2726.7901513428628</v>
+        <v>-6075.7997198114126</v>
       </c>
       <c r="AD10">
         <f t="shared" si="15"/>
-        <v>3858.7236586837598</v>
+        <v>-4943.8662124705161</v>
       </c>
       <c r="AE10">
         <f t="shared" si="16"/>
-        <v>45219.641193982869</v>
+        <v>36417.051322828593</v>
       </c>
       <c r="AF10">
         <f t="shared" si="17"/>
-        <v>2353.9574530792438</v>
+        <v>-6448.6324180750307</v>
       </c>
       <c r="AG10">
         <f t="shared" si="18"/>
-        <v>3371.689953744798</v>
+        <v>-5430.899917409477</v>
       </c>
       <c r="AH10">
         <f t="shared" si="19"/>
-        <v>40597.859276769006</v>
-      </c>
-    </row>
-    <row r="11" spans="1:34" x14ac:dyDescent="0.3">
+        <v>31795.269405614723</v>
+      </c>
+    </row>
+    <row r="11" spans="1:34" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A11" s="1">
         <v>2027</v>
       </c>
@@ -17890,31 +17809,31 @@
       </c>
       <c r="U11">
         <f>OPEX!$B$3</f>
-        <v>2139.68314436323</v>
+        <v>21008.816291188887</v>
       </c>
       <c r="V11">
         <f t="shared" si="8"/>
-        <v>8725.1168556367702</v>
+        <v>-10144.016291188886</v>
       </c>
       <c r="W11">
         <f t="shared" si="9"/>
-        <v>12461.916855636769</v>
+        <v>-6407.2162911888863</v>
       </c>
       <c r="X11">
         <f t="shared" si="1"/>
-        <v>138382.71685563677</v>
+        <v>119513.58370881111</v>
       </c>
       <c r="Y11">
         <f t="shared" si="10"/>
-        <v>7637.9168556367704</v>
+        <v>-11231.216291188886</v>
       </c>
       <c r="Z11">
         <f t="shared" si="11"/>
-        <v>11000.316855636771</v>
+        <v>-7868.8162911888867</v>
       </c>
       <c r="AA11">
         <f t="shared" si="12"/>
-        <v>124328.31685563677</v>
+        <v>105459.18370881112</v>
       </c>
       <c r="AB11">
         <f t="shared" si="13"/>
@@ -17922,30 +17841,30 @@
       </c>
       <c r="AC11">
         <f t="shared" si="14"/>
-        <v>3700.3012784971766</v>
+        <v>-4302.0531498248911</v>
       </c>
       <c r="AD11">
         <f t="shared" si="15"/>
-        <v>5285.0692588314769</v>
+        <v>-2717.2851694905908</v>
       </c>
       <c r="AE11">
         <f t="shared" si="16"/>
-        <v>58687.780642389444</v>
+        <v>50685.426214067375</v>
       </c>
       <c r="AF11">
         <f t="shared" si="17"/>
-        <v>3239.2223478026112</v>
+        <v>-4763.1320805194573</v>
       </c>
       <c r="AG11">
         <f t="shared" si="18"/>
-        <v>4665.2081798182535</v>
+        <v>-3337.1462485038146</v>
       </c>
       <c r="AH11">
         <f t="shared" si="19"/>
-        <v>52727.343074735196</v>
-      </c>
-    </row>
-    <row r="12" spans="1:34" x14ac:dyDescent="0.3">
+        <v>44724.988646413127</v>
+      </c>
+    </row>
+    <row r="12" spans="1:34" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A12" s="1">
         <v>2028</v>
       </c>
@@ -17999,31 +17918,31 @@
       </c>
       <c r="U12">
         <f>OPEX!$B$3</f>
-        <v>2139.68314436323</v>
+        <v>21008.816291188887</v>
       </c>
       <c r="V12">
         <f t="shared" si="8"/>
-        <v>12577.11685563677</v>
+        <v>-6292.0162911888856</v>
       </c>
       <c r="W12">
         <f t="shared" si="9"/>
-        <v>18178.716855636772</v>
+        <v>-690.41629118888522</v>
       </c>
       <c r="X12">
         <f t="shared" si="1"/>
-        <v>163265.91685563678</v>
+        <v>144396.78370881113</v>
       </c>
       <c r="Y12">
         <f t="shared" si="10"/>
-        <v>11101.11685563677</v>
+        <v>-7768.0162911888856</v>
       </c>
       <c r="Z12">
         <f t="shared" si="11"/>
-        <v>16141.11685563677</v>
+        <v>-2728.0162911888874</v>
       </c>
       <c r="AA12">
         <f t="shared" si="12"/>
-        <v>146720.31685563677</v>
+        <v>127851.18370881112</v>
       </c>
       <c r="AB12">
         <f t="shared" si="13"/>
@@ -18031,30 +17950,30 @@
       </c>
       <c r="AC12">
         <f t="shared" si="14"/>
-        <v>4849.0230040618062</v>
+        <v>-2425.8446580491636</v>
       </c>
       <c r="AD12">
         <f t="shared" si="15"/>
-        <v>7008.6822941302707</v>
+        <v>-266.18536798070005</v>
       </c>
       <c r="AE12">
         <f t="shared" si="16"/>
-        <v>62946.07863625059</v>
+        <v>55671.210974139627</v>
       </c>
       <c r="AF12">
         <f t="shared" si="17"/>
-        <v>4279.9611088638176</v>
+        <v>-2994.9065532471523</v>
       </c>
       <c r="AG12">
         <f t="shared" si="18"/>
-        <v>6223.0992875886559</v>
+        <v>-1051.7683745223142</v>
       </c>
       <c r="AH12">
         <f t="shared" si="19"/>
-        <v>56567.033586665333</v>
-      </c>
-    </row>
-    <row r="13" spans="1:34" x14ac:dyDescent="0.3">
+        <v>49292.165924554363</v>
+      </c>
+    </row>
+    <row r="13" spans="1:34" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A13" s="1">
         <v>2029</v>
       </c>
@@ -18107,31 +18026,31 @@
       </c>
       <c r="U13">
         <f>OPEX!$B$3</f>
-        <v>2139.68314436323</v>
+        <v>21008.816291188887</v>
       </c>
       <c r="V13">
         <f t="shared" si="8"/>
-        <v>17667.516855636772</v>
+        <v>-1201.616291188886</v>
       </c>
       <c r="W13">
         <f t="shared" si="9"/>
-        <v>25846.716855636772</v>
+        <v>6977.5837088111148</v>
       </c>
       <c r="X13">
         <f t="shared" si="1"/>
-        <v>168593.91685563678</v>
+        <v>149724.78370881113</v>
       </c>
       <c r="Y13">
         <f t="shared" si="10"/>
-        <v>15680.316855636771</v>
+        <v>-3188.8162911888867</v>
       </c>
       <c r="Z13">
         <f t="shared" si="11"/>
-        <v>23045.916855636773</v>
+        <v>4176.7837088111155</v>
       </c>
       <c r="AA13">
         <f t="shared" si="12"/>
-        <v>151515.51685563679</v>
+        <v>132646.38370881113</v>
       </c>
       <c r="AB13">
         <f t="shared" si="13"/>
@@ -18139,30 +18058,30 @@
       </c>
       <c r="AC13">
         <f t="shared" si="14"/>
-        <v>6192.3568768853575</v>
+        <v>-421.15917957916071</v>
       </c>
       <c r="AD13">
         <f t="shared" si="15"/>
-        <v>9059.1165795235611</v>
+        <v>2445.6005230590426</v>
       </c>
       <c r="AE13">
         <f t="shared" si="16"/>
-        <v>59091.13934757375</v>
+        <v>52477.623291109237</v>
       </c>
       <c r="AF13">
         <f t="shared" si="17"/>
-        <v>5495.8553998359339</v>
+        <v>-1117.6606566285836</v>
       </c>
       <c r="AG13">
         <f t="shared" si="18"/>
-        <v>8077.4532658560775</v>
+        <v>1463.9372093915597</v>
       </c>
       <c r="AH13">
         <f t="shared" si="19"/>
-        <v>53105.264334670748</v>
-      </c>
-    </row>
-    <row r="14" spans="1:34" x14ac:dyDescent="0.3">
+        <v>46491.748278206229</v>
+      </c>
+    </row>
+    <row r="14" spans="1:34" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A14" s="1">
         <v>2030</v>
       </c>
@@ -18209,31 +18128,31 @@
       </c>
       <c r="U14">
         <f>OPEX!$B$3</f>
-        <v>2139.68314436323</v>
+        <v>21008.816291188887</v>
       </c>
       <c r="V14">
         <f t="shared" si="8"/>
-        <v>24298.716855636772</v>
+        <v>5429.5837088111148</v>
       </c>
       <c r="W14">
         <f t="shared" si="9"/>
-        <v>35883.516855636772</v>
+        <v>17014.383708811118</v>
       </c>
       <c r="X14">
         <f t="shared" si="1"/>
-        <v>168838.71685563677</v>
+        <v>149969.58370881111</v>
       </c>
       <c r="Y14">
         <f t="shared" si="10"/>
-        <v>21649.11685563677</v>
+        <v>2779.9837088111126</v>
       </c>
       <c r="Z14">
         <f t="shared" si="11"/>
-        <v>32074.716855636772</v>
+        <v>13205.583708811115</v>
       </c>
       <c r="AA14">
         <f t="shared" si="12"/>
-        <v>151738.71685563677</v>
+        <v>132869.58370881111</v>
       </c>
       <c r="AB14">
         <f t="shared" si="13"/>
@@ -18241,30 +18160,30 @@
       </c>
       <c r="AC14">
         <f t="shared" si="14"/>
-        <v>7742.3200210239684</v>
+        <v>1730.0326969653161</v>
       </c>
       <c r="AD14">
         <f t="shared" si="15"/>
-        <v>11433.594318034908</v>
+        <v>5421.3069939762554</v>
       </c>
       <c r="AE14">
         <f t="shared" si="16"/>
-        <v>53797.218412878909</v>
+        <v>47784.931088820253</v>
       </c>
       <c r="AF14">
         <f t="shared" si="17"/>
-        <v>6898.0758064186075</v>
+        <v>885.78848235995463</v>
       </c>
       <c r="AG14">
         <f t="shared" si="18"/>
-        <v>10219.993259539702</v>
+        <v>4207.705935481049</v>
       </c>
       <c r="AH14">
         <f t="shared" si="19"/>
-        <v>48348.631430031804</v>
-      </c>
-    </row>
-    <row r="15" spans="1:34" x14ac:dyDescent="0.3">
+        <v>42336.344105973156</v>
+      </c>
+    </row>
+    <row r="15" spans="1:34" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A15" s="1">
         <v>2031</v>
       </c>
@@ -18311,31 +18230,31 @@
       </c>
       <c r="U15">
         <f>OPEX!$B$3</f>
-        <v>2139.68314436323</v>
+        <v>21008.816291188887</v>
       </c>
       <c r="V15">
         <f t="shared" si="8"/>
-        <v>32773.11685563677</v>
+        <v>13903.983708811116</v>
       </c>
       <c r="W15">
         <f t="shared" si="9"/>
-        <v>48562.716855636769</v>
+        <v>29693.583708811115</v>
       </c>
       <c r="X15">
         <f t="shared" si="1"/>
-        <v>168881.91685563678</v>
+        <v>150012.78370881113</v>
       </c>
       <c r="Y15">
         <f t="shared" si="10"/>
-        <v>29281.11685563677</v>
+        <v>10411.983708811113</v>
       </c>
       <c r="Z15">
         <f t="shared" si="11"/>
-        <v>43486.716855636769</v>
+        <v>24617.583708811115</v>
       </c>
       <c r="AA15">
         <f t="shared" si="12"/>
-        <v>151774.71685563677</v>
+        <v>132905.58370881111</v>
       </c>
       <c r="AB15">
         <f t="shared" si="13"/>
@@ -18343,30 +18262,30 @@
       </c>
       <c r="AC15">
         <f t="shared" si="14"/>
-        <v>9493.2045660260137</v>
+        <v>4027.4888168817838</v>
       </c>
       <c r="AD15">
         <f t="shared" si="15"/>
-        <v>14066.889256316417</v>
+        <v>8601.1735071721887</v>
       </c>
       <c r="AE15">
         <f t="shared" si="16"/>
-        <v>48919.075694730906</v>
+        <v>43453.359945586679</v>
       </c>
       <c r="AF15">
         <f t="shared" si="17"/>
-        <v>8481.6965519854984</v>
+        <v>3015.980802841269</v>
       </c>
       <c r="AG15">
         <f t="shared" si="18"/>
-        <v>12596.552864772992</v>
+        <v>7130.8371156287621</v>
       </c>
       <c r="AH15">
         <f t="shared" si="19"/>
-        <v>43963.729217699438</v>
-      </c>
-    </row>
-    <row r="16" spans="1:34" x14ac:dyDescent="0.3">
+        <v>38498.013468555211</v>
+      </c>
+    </row>
+    <row r="16" spans="1:34" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A16" s="1">
         <v>2032</v>
       </c>
@@ -18413,31 +18332,31 @@
       </c>
       <c r="U16">
         <f>OPEX!$B$3</f>
-        <v>2139.68314436323</v>
+        <v>21008.816291188887</v>
       </c>
       <c r="V16">
         <f t="shared" si="8"/>
-        <v>43299.516855636772</v>
+        <v>24430.383708811118</v>
       </c>
       <c r="W16">
         <f t="shared" si="9"/>
-        <v>63855.516855636764</v>
+        <v>44986.38370881111</v>
       </c>
       <c r="X16">
         <f t="shared" si="1"/>
-        <v>168903.51685563679</v>
+        <v>150034.38370881113</v>
       </c>
       <c r="Y16">
         <f t="shared" si="10"/>
-        <v>38749.11685563677</v>
+        <v>19879.983708811116</v>
       </c>
       <c r="Z16">
         <f t="shared" si="11"/>
-        <v>57253.11685563677</v>
+        <v>38383.983708811116</v>
       </c>
       <c r="AA16">
         <f t="shared" si="12"/>
-        <v>151796.31685563677</v>
+        <v>132927.18370881112</v>
       </c>
       <c r="AB16">
         <f t="shared" si="13"/>
@@ -18445,30 +18364,30 @@
       </c>
       <c r="AC16">
         <f t="shared" si="14"/>
-        <v>11402.116084442072</v>
+        <v>6433.2835852200478</v>
       </c>
       <c r="AD16">
         <f t="shared" si="15"/>
-        <v>16815.153347957847</v>
+        <v>11846.320848735821</v>
       </c>
       <c r="AE16">
         <f t="shared" si="16"/>
-        <v>44477.574950302915</v>
+        <v>39508.742451080892</v>
       </c>
       <c r="AF16">
         <f t="shared" si="17"/>
-        <v>10203.853544847687</v>
+        <v>5235.0210456256618</v>
       </c>
       <c r="AG16">
         <f t="shared" si="18"/>
-        <v>15076.535074527386</v>
+        <v>10107.702575305362</v>
       </c>
       <c r="AH16">
         <f t="shared" si="19"/>
-        <v>39972.714516637941</v>
-      </c>
-    </row>
-    <row r="17" spans="1:34" x14ac:dyDescent="0.3">
+        <v>35003.882017415919</v>
+      </c>
+    </row>
+    <row r="17" spans="1:34" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A17" s="1">
         <v>2033</v>
       </c>
@@ -18515,31 +18434,31 @@
       </c>
       <c r="U17">
         <f>OPEX!$B$3</f>
-        <v>2139.68314436323</v>
+        <v>21008.816291188887</v>
       </c>
       <c r="V17">
         <f t="shared" si="8"/>
-        <v>55949.916855636766</v>
+        <v>37080.783708811112</v>
       </c>
       <c r="W17">
         <f t="shared" si="9"/>
-        <v>81236.316855636775</v>
+        <v>62367.183708811113</v>
       </c>
       <c r="X17">
         <f t="shared" si="1"/>
-        <v>168917.91685563678</v>
+        <v>150048.78370881113</v>
       </c>
       <c r="Y17">
         <f t="shared" si="10"/>
-        <v>50139.516855636772</v>
+        <v>31270.383708811118</v>
       </c>
       <c r="Z17">
         <f t="shared" si="11"/>
-        <v>72898.716855636783</v>
+        <v>54029.583708811122</v>
       </c>
       <c r="AA17">
         <f t="shared" si="12"/>
-        <v>151810.71685563677</v>
+        <v>132941.58370881111</v>
       </c>
       <c r="AB17">
         <f t="shared" si="13"/>
@@ -18547,30 +18466,30 @@
       </c>
       <c r="AC17">
         <f t="shared" si="14"/>
-        <v>13393.965258105183</v>
+        <v>8876.8448042669788</v>
       </c>
       <c r="AD17">
         <f t="shared" si="15"/>
-        <v>19447.328375273599</v>
+        <v>14930.207921435393</v>
       </c>
       <c r="AE17">
         <f t="shared" si="16"/>
-        <v>40437.606291240838</v>
+        <v>35920.48583740263</v>
       </c>
       <c r="AF17">
         <f t="shared" si="17"/>
-        <v>12003.001694450599</v>
+        <v>7485.8812406123934</v>
       </c>
       <c r="AG17">
         <f t="shared" si="18"/>
-        <v>17451.373224453266</v>
+        <v>12934.252770615058</v>
       </c>
       <c r="AH17">
         <f t="shared" si="19"/>
-        <v>36342.27862427268</v>
-      </c>
-    </row>
-    <row r="18" spans="1:34" x14ac:dyDescent="0.3">
+        <v>31825.158170434479</v>
+      </c>
+    </row>
+    <row r="18" spans="1:34" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A18" s="1">
         <v>2034</v>
       </c>
@@ -18617,31 +18536,31 @@
       </c>
       <c r="U18">
         <f>OPEX!$B$3</f>
-        <v>2139.68314436323</v>
+        <v>21008.816291188887</v>
       </c>
       <c r="V18">
         <f t="shared" si="8"/>
-        <v>70486.716855636783</v>
+        <v>51617.583708811122</v>
       </c>
       <c r="W18">
         <f t="shared" si="9"/>
-        <v>99567.516855636772</v>
+        <v>80698.383708811103</v>
       </c>
       <c r="X18">
         <f t="shared" si="1"/>
-        <v>168925.11685563679</v>
+        <v>150055.98370881114</v>
       </c>
       <c r="Y18">
         <f t="shared" si="10"/>
-        <v>63221.916855636766</v>
+        <v>44352.783708811112</v>
       </c>
       <c r="Z18">
         <f t="shared" si="11"/>
-        <v>89393.91685563678</v>
+        <v>70524.783708811126</v>
       </c>
       <c r="AA18">
         <f t="shared" si="12"/>
-        <v>151817.91685563678</v>
+        <v>132948.78370881113</v>
       </c>
       <c r="AB18">
         <f t="shared" si="13"/>
@@ -18649,30 +18568,30 @@
       </c>
       <c r="AC18">
         <f t="shared" si="14"/>
-        <v>15339.96327397713</v>
+        <v>11233.490134124215</v>
       </c>
       <c r="AD18">
         <f t="shared" si="15"/>
-        <v>21668.792646063277</v>
+        <v>17562.319506210362</v>
       </c>
       <c r="AE18">
         <f t="shared" si="16"/>
-        <v>36763.02719454209</v>
+        <v>32656.554054689175</v>
       </c>
       <c r="AF18">
         <f t="shared" si="17"/>
-        <v>13758.931128288854</v>
+        <v>9652.4579884359409</v>
       </c>
       <c r="AG18">
         <f t="shared" si="18"/>
-        <v>19454.720870188623</v>
+        <v>15348.247730335712</v>
       </c>
       <c r="AH18">
         <f t="shared" si="19"/>
-        <v>33040.002042752858</v>
-      </c>
-    </row>
-    <row r="19" spans="1:34" x14ac:dyDescent="0.3">
+        <v>28933.528902899943</v>
+      </c>
+    </row>
+    <row r="19" spans="1:34" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A19" s="1">
         <v>2035</v>
       </c>
@@ -18719,31 +18638,31 @@
       </c>
       <c r="U19">
         <f>OPEX!$B$3</f>
-        <v>2139.68314436323</v>
+        <v>21008.816291188887</v>
       </c>
       <c r="V19">
         <f t="shared" si="8"/>
-        <v>86326.716855636783</v>
+        <v>67457.583708811115</v>
       </c>
       <c r="W19">
         <f t="shared" si="9"/>
-        <v>117250.71685563678</v>
+        <v>98381.583708811115</v>
       </c>
       <c r="X19">
         <f t="shared" si="1"/>
-        <v>168925.11685563679</v>
+        <v>150055.98370881114</v>
       </c>
       <c r="Y19">
         <f t="shared" si="10"/>
-        <v>77477.91685563678</v>
+        <v>58608.783708811119</v>
       </c>
       <c r="Z19">
         <f t="shared" si="11"/>
-        <v>105305.91685563678</v>
+        <v>86436.783708811126</v>
       </c>
       <c r="AA19">
         <f t="shared" si="12"/>
-        <v>151817.91685563678</v>
+        <v>132948.78370881113</v>
       </c>
       <c r="AB19">
         <f t="shared" si="13"/>
@@ -18751,30 +18670,30 @@
       </c>
       <c r="AC19">
         <f t="shared" si="14"/>
-        <v>17079.280713539163</v>
+        <v>13346.123313672877</v>
       </c>
       <c r="AD19">
         <f t="shared" si="15"/>
-        <v>23197.429254606941</v>
+        <v>19464.271854740651</v>
       </c>
       <c r="AE19">
         <f t="shared" si="16"/>
-        <v>33420.933813220079</v>
+        <v>29687.776413353793</v>
       </c>
       <c r="AF19">
         <f t="shared" si="17"/>
-        <v>15328.592807375649</v>
+        <v>11595.435407509363</v>
       </c>
       <c r="AG19">
         <f t="shared" si="18"/>
-        <v>20834.214253528608</v>
+        <v>17101.056853662321</v>
       </c>
       <c r="AH19">
         <f t="shared" si="19"/>
-        <v>30036.365493411686</v>
-      </c>
-    </row>
-    <row r="20" spans="1:34" x14ac:dyDescent="0.3">
+        <v>26303.208093545403</v>
+      </c>
+    </row>
+    <row r="20" spans="1:34" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A20" s="1">
         <v>2036</v>
       </c>
@@ -18821,31 +18740,31 @@
       </c>
       <c r="U20">
         <f>OPEX!$B$3</f>
-        <v>2139.68314436323</v>
+        <v>21008.816291188887</v>
       </c>
       <c r="V20">
         <f t="shared" si="8"/>
-        <v>102512.31685563677</v>
+        <v>83643.183708811121</v>
       </c>
       <c r="W20">
         <f t="shared" si="9"/>
-        <v>132716.31685563677</v>
+        <v>113847.18370881112</v>
       </c>
       <c r="X20">
         <f t="shared" si="1"/>
-        <v>168932.31685563677</v>
+        <v>150063.18370881112</v>
       </c>
       <c r="Y20">
         <f t="shared" si="10"/>
-        <v>92043.516855636772</v>
+        <v>73174.383708811103</v>
       </c>
       <c r="Z20">
         <f t="shared" si="11"/>
-        <v>119230.71685563678</v>
+        <v>100361.58370881111</v>
       </c>
       <c r="AA20">
         <f t="shared" si="12"/>
-        <v>151825.11685563679</v>
+        <v>132955.98370881114</v>
       </c>
       <c r="AB20">
         <f t="shared" si="13"/>
@@ -18853,30 +18772,30 @@
       </c>
       <c r="AC20">
         <f t="shared" si="14"/>
-        <v>18437.741260444716</v>
+        <v>15043.961806020819</v>
       </c>
       <c r="AD20">
         <f t="shared" si="15"/>
-        <v>23870.196150862605</v>
+        <v>20476.416696438708</v>
       </c>
       <c r="AE20">
         <f t="shared" si="16"/>
-        <v>30383.962086214684</v>
+        <v>26990.182631790791</v>
       </c>
       <c r="AF20">
         <f t="shared" si="17"/>
-        <v>16554.83556064314</v>
+        <v>13161.056106219241</v>
       </c>
       <c r="AG20">
         <f t="shared" si="18"/>
-        <v>21444.692453662912</v>
+        <v>18050.912999239015</v>
       </c>
       <c r="AH20">
         <f t="shared" si="19"/>
-        <v>27307.081795479789</v>
-      </c>
-    </row>
-    <row r="21" spans="1:34" x14ac:dyDescent="0.3">
+        <v>23913.302341055893</v>
+      </c>
+    </row>
+    <row r="21" spans="1:34" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A21" s="1">
         <v>2037</v>
       </c>
@@ -18923,31 +18842,31 @@
       </c>
       <c r="U21">
         <f>OPEX!$B$3</f>
-        <v>2139.68314436323</v>
+        <v>21008.816291188887</v>
       </c>
       <c r="V21">
         <f t="shared" si="8"/>
-        <v>117913.11685563678</v>
+        <v>99043.983708811109</v>
       </c>
       <c r="W21">
         <f t="shared" si="9"/>
-        <v>144963.51685563679</v>
+        <v>126094.38370881113</v>
       </c>
       <c r="X21">
         <f t="shared" si="1"/>
-        <v>168932.31685563677</v>
+        <v>150063.18370881112</v>
       </c>
       <c r="Y21">
         <f t="shared" si="10"/>
-        <v>105903.51685563677</v>
+        <v>87034.383708811103</v>
       </c>
       <c r="Z21">
         <f t="shared" si="11"/>
-        <v>130246.71685563677</v>
+        <v>111377.58370881111</v>
       </c>
       <c r="AA21">
         <f t="shared" si="12"/>
-        <v>151825.11685563679</v>
+        <v>132955.98370881114</v>
       </c>
       <c r="AB21">
         <f t="shared" si="13"/>
@@ -18955,30 +18874,30 @@
       </c>
       <c r="AC21">
         <f t="shared" si="14"/>
-        <v>19279.736829162299</v>
+        <v>16194.482779686028</v>
       </c>
       <c r="AD21">
         <f t="shared" si="15"/>
-        <v>23702.693384217018</v>
+        <v>20617.439334740753</v>
       </c>
       <c r="AE21">
         <f t="shared" si="16"/>
-        <v>27621.783714740617</v>
+        <v>24536.529665264348</v>
       </c>
       <c r="AF21">
         <f t="shared" si="17"/>
-        <v>17316.071262531666</v>
+        <v>14230.817213055399</v>
       </c>
       <c r="AG21">
         <f t="shared" si="18"/>
-        <v>21296.378984820731</v>
+        <v>18211.124935344462</v>
       </c>
       <c r="AH21">
         <f t="shared" si="19"/>
-        <v>24824.619814072528</v>
-      </c>
-    </row>
-    <row r="22" spans="1:34" x14ac:dyDescent="0.3">
+        <v>21739.365764596263</v>
+      </c>
+    </row>
+    <row r="22" spans="1:34" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A22" s="1">
         <v>2038</v>
       </c>
@@ -19025,31 +18944,31 @@
       </c>
       <c r="U22">
         <f>OPEX!$B$3</f>
-        <v>2139.68314436323</v>
+        <v>21008.816291188887</v>
       </c>
       <c r="V22">
         <f t="shared" si="8"/>
-        <v>131485.11685563679</v>
+        <v>112615.98370881114</v>
       </c>
       <c r="W22">
         <f t="shared" si="9"/>
-        <v>153797.91685563678</v>
+        <v>134928.78370881113</v>
       </c>
       <c r="X22">
         <f t="shared" si="1"/>
-        <v>168932.31685563677</v>
+        <v>150063.18370881112</v>
       </c>
       <c r="Y22">
         <f t="shared" si="10"/>
-        <v>118121.91685563678</v>
+        <v>99252.783708811126</v>
       </c>
       <c r="Z22">
         <f t="shared" si="11"/>
-        <v>138202.71685563677</v>
+        <v>119333.58370881111</v>
       </c>
       <c r="AA22">
         <f t="shared" si="12"/>
-        <v>151825.11685563679</v>
+        <v>132955.98370881114</v>
       </c>
       <c r="AB22">
         <f t="shared" si="13"/>
@@ -19057,30 +18976,30 @@
       </c>
       <c r="AC22">
         <f t="shared" si="14"/>
-        <v>19544.424800600314</v>
+        <v>16739.648391985527</v>
       </c>
       <c r="AD22">
         <f t="shared" si="15"/>
-        <v>22861.080343977421</v>
+        <v>20056.303935362634</v>
       </c>
       <c r="AE22">
         <f t="shared" si="16"/>
-        <v>25110.712467946018</v>
+        <v>22305.93605933123</v>
       </c>
       <c r="AF22">
         <f t="shared" si="17"/>
-        <v>17558.070270588079</v>
+        <v>14753.29386197329</v>
       </c>
       <c r="AG22">
         <f t="shared" si="18"/>
-        <v>20542.953236215297</v>
+        <v>17738.17682760051</v>
       </c>
       <c r="AH22">
         <f t="shared" si="19"/>
-        <v>22567.836194611395</v>
-      </c>
-    </row>
-    <row r="25" spans="1:34" x14ac:dyDescent="0.3">
+        <v>19763.059785996604</v>
+      </c>
+    </row>
+    <row r="25" spans="1:34" ht="14.45" x14ac:dyDescent="0.3">
       <c r="I25" t="s">
         <v>29</v>
       </c>
@@ -19094,7 +19013,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="28" spans="1:34" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:34" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>25</v>
       </c>
@@ -19117,7 +19036,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="29" spans="1:34" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:34" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A29" s="1">
         <v>2018</v>
       </c>
@@ -19146,7 +19065,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="30" spans="1:34" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:34" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A30" s="1">
         <v>2019</v>
       </c>
@@ -19175,7 +19094,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="31" spans="1:34" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:34" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A31" s="1">
         <v>2020</v>
       </c>
@@ -19204,7 +19123,7 @@
         <v>307</v>
       </c>
     </row>
-    <row r="32" spans="1:34" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:34" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A32" s="1">
         <v>2021</v>
       </c>
@@ -19233,7 +19152,7 @@
         <v>594</v>
       </c>
     </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A33" s="1">
         <v>2022</v>
       </c>
@@ -19262,7 +19181,7 @@
         <v>1155</v>
       </c>
     </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A34" s="1">
         <v>2023</v>
       </c>
@@ -19291,7 +19210,7 @@
         <v>2225</v>
       </c>
     </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A35" s="1">
         <v>2024</v>
       </c>
@@ -19320,7 +19239,7 @@
         <v>4194</v>
       </c>
     </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A36" s="1">
         <v>2025</v>
       </c>
@@ -19349,7 +19268,7 @@
         <v>7535</v>
       </c>
     </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A37" s="1">
         <v>2026</v>
       </c>
@@ -19378,7 +19297,7 @@
         <v>12384</v>
       </c>
     </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A38" s="1">
         <v>2027</v>
       </c>
@@ -19407,7 +19326,7 @@
         <v>17565</v>
       </c>
     </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A39" s="1">
         <v>2028</v>
       </c>
@@ -19436,7 +19355,7 @@
         <v>20675</v>
       </c>
     </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A40" s="1">
         <v>2029</v>
       </c>
@@ -19465,7 +19384,7 @@
         <v>21341</v>
       </c>
     </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A41" s="1">
         <v>2030</v>
       </c>
@@ -19494,7 +19413,7 @@
         <v>21372</v>
       </c>
     </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A42" s="1">
         <v>2031</v>
       </c>
@@ -19523,7 +19442,7 @@
         <v>21377</v>
       </c>
     </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A43" s="1">
         <v>2032</v>
       </c>
@@ -19552,7 +19471,7 @@
         <v>21380</v>
       </c>
     </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A44" s="1">
         <v>2033</v>
       </c>
@@ -19581,7 +19500,7 @@
         <v>21382</v>
       </c>
     </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A45" s="1">
         <v>2034</v>
       </c>
@@ -19610,7 +19529,7 @@
         <v>21383</v>
       </c>
     </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A46" s="1">
         <v>2035</v>
       </c>
@@ -19639,7 +19558,7 @@
         <v>21383</v>
       </c>
     </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A47" s="1">
         <v>2036</v>
       </c>
@@ -19668,7 +19587,7 @@
         <v>21384</v>
       </c>
     </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A48" s="1">
         <v>2037</v>
       </c>
@@ -19697,7 +19616,7 @@
         <v>21384</v>
       </c>
     </row>
-    <row r="49" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A49" s="1">
         <v>2038</v>
       </c>
@@ -19743,9 +19662,9 @@
       <selection activeCell="A17" sqref="A17:XFD17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="19" max="19" width="14.88671875" customWidth="1"/>
+    <col min="19" max="19" width="14.85546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:21" x14ac:dyDescent="0.3">
@@ -21195,7 +21114,7 @@
       <selection activeCell="B17" sqref="B17:L17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
@@ -22644,7 +22563,7 @@
       <selection activeCell="I47" sqref="I47"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
@@ -24093,7 +24012,7 @@
       <selection activeCell="L29" sqref="L29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
@@ -25542,7 +25461,7 @@
       <selection activeCell="L27" sqref="L27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
@@ -26991,7 +26910,7 @@
       <selection activeCell="I33" sqref="I33"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A1" t="s">

</xml_diff>